<commit_message>
Created functions to make and utilize turbine dictionary
</commit_message>
<xml_diff>
--- a/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
+++ b/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="705" windowWidth="17565" windowHeight="12990" activeTab="1"/>
+    <workbookView xWindow="1560" yWindow="705" windowWidth="17565" windowHeight="12990"/>
   </bookViews>
   <sheets>
     <sheet name="Main Page" sheetId="5" r:id="rId1"/>
-    <sheet name="Blade_JR" sheetId="9" r:id="rId2"/>
-    <sheet name="Tower Data" sheetId="4" r:id="rId3"/>
-    <sheet name="Blade Data" sheetId="3" r:id="rId4"/>
-    <sheet name="GECbladedata" sheetId="6" r:id="rId5"/>
-    <sheet name="GECtwrdata" sheetId="7" r:id="rId6"/>
-    <sheet name="GECdrivetrain" sheetId="8" r:id="rId7"/>
+    <sheet name="Rotor_JR" sheetId="9" r:id="rId2"/>
+    <sheet name="Nacelle_JR" sheetId="10" r:id="rId3"/>
+    <sheet name="Tower Data" sheetId="4" r:id="rId4"/>
+    <sheet name="Blade Data" sheetId="3" r:id="rId5"/>
+    <sheet name="GECbladedata" sheetId="6" r:id="rId6"/>
+    <sheet name="GECtwrdata" sheetId="7" r:id="rId7"/>
+    <sheet name="GECdrivetrain" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Blade Data'!$A$6:$Q$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Blade Data'!$A$6:$Q$32</definedName>
   </definedNames>
   <calcPr calcId="145621" iterate="1" iterateDelta="1E-4"/>
 </workbook>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="410">
   <si>
     <t>number</t>
   </si>
@@ -1719,10 +1720,10 @@
     <t>&lt;--- AFName changed to match documentation/avaialble airfoils</t>
   </si>
   <si>
-    <t>EIEdge</t>
-  </si>
-  <si>
-    <t>EIFlap</t>
+    <t>blade modal damping ratios</t>
+  </si>
+  <si>
+    <t>Cylinder changed to produce correct AeroCent</t>
   </si>
 </sst>
 </file>
@@ -1736,7 +1737,7 @@
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="36">
     <font>
       <sz val="8"/>
       <name val="Arial"/>
@@ -1951,13 +1952,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -2003,7 +1997,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -2562,12 +2556,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="375">
+  <cellXfs count="374">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3363,16 +3383,16 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3401,9 +3421,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3413,12 +3430,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3601,19 +3616,19 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.33741427482854974</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.33741427482854963</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4771354983247496E-2</c:v>
+                  <c:v>0.29594991734037218</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.9390279955326658E-2</c:v>
+                  <c:v>0.22684265486007649</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.4009204927405833E-2</c:v>
+                  <c:v>0.15773539237978068</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>8.8628129899484986E-2</c:v>
@@ -3764,19 +3779,19 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.33741427482854974</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.33741427482854963</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.6555553178479854E-3</c:v>
+                  <c:v>0.27552300703927668</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.5081480847594629E-2</c:v>
+                  <c:v>0.17237089405715517</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.4507406377341275E-2</c:v>
+                  <c:v>6.9218781075033597E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-3.3933331907087916E-2</c:v>
@@ -4002,11 +4017,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81605376"/>
-        <c:axId val="81607296"/>
+        <c:axId val="82432768"/>
+        <c:axId val="82434688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81605376"/>
+        <c:axId val="82432768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4091,12 +4106,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81607296"/>
+        <c:crossAx val="82434688"/>
         <c:crossesAt val="-10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81607296"/>
+        <c:axId val="82434688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4180,7 +4195,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81605376"/>
+        <c:crossAx val="82432768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4730,6 +4745,18 @@
             </a:rPr>
             <a:t>                        report and available airfoils (JRinker)</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                          Changed AC for cylinders to yield correct AeroCent</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1000">
             <a:effectLst/>
           </a:endParaRPr>
@@ -5227,10 +5254,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U138"/>
+  <dimension ref="A1:U142"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H123" sqref="H123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -5254,14 +5281,14 @@
       <c r="B1" s="337" t="s">
         <v>401</v>
       </c>
-      <c r="C1" s="363" t="s">
+      <c r="C1" s="365" t="s">
         <v>402</v>
       </c>
-      <c r="D1" s="364"/>
-      <c r="E1" s="364"/>
-      <c r="F1" s="364"/>
-      <c r="G1" s="364"/>
-      <c r="H1" s="365"/>
+      <c r="D1" s="366"/>
+      <c r="E1" s="366"/>
+      <c r="F1" s="366"/>
+      <c r="G1" s="366"/>
+      <c r="H1" s="367"/>
     </row>
     <row r="2" spans="1:8" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="A2" s="60" t="s">
@@ -5277,17 +5304,17 @@
       <c r="A3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="357" t="s">
+      <c r="B3" s="359" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="358"/>
-      <c r="D3" s="359"/>
+      <c r="C3" s="360"/>
+      <c r="D3" s="361"/>
       <c r="E3" s="35"/>
-      <c r="F3" s="360" t="s">
+      <c r="F3" s="362" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="361"/>
-      <c r="H3" s="362"/>
+      <c r="G3" s="363"/>
+      <c r="H3" s="364"/>
     </row>
     <row r="4" spans="1:8" ht="12" thickBot="1">
       <c r="A4" s="20" t="s">
@@ -5550,11 +5577,11 @@
       <c r="C18" s="330">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D18" s="366" t="s">
+      <c r="D18" s="368" t="s">
         <v>374</v>
       </c>
-      <c r="E18" s="365"/>
-      <c r="F18" s="365"/>
+      <c r="E18" s="367"/>
+      <c r="F18" s="367"/>
     </row>
     <row r="19" spans="1:21" ht="25.5" customHeight="1">
       <c r="A19" s="267" t="s">
@@ -5566,11 +5593,11 @@
       <c r="C19" s="330">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D19" s="366" t="s">
+      <c r="D19" s="368" t="s">
         <v>373</v>
       </c>
-      <c r="E19" s="365"/>
-      <c r="F19" s="365"/>
+      <c r="E19" s="367"/>
+      <c r="F19" s="367"/>
       <c r="I19" s="35" t="s">
         <v>69</v>
       </c>
@@ -6717,8 +6744,8 @@
       <c r="D115" s="304" t="s">
         <v>378</v>
       </c>
-      <c r="E115" s="305">
-        <v>0.5</v>
+      <c r="E115" s="373">
+        <v>0.25</v>
       </c>
       <c r="F115" s="303">
         <v>0.5</v>
@@ -6758,8 +6785,8 @@
       <c r="D116" s="310" t="s">
         <v>378</v>
       </c>
-      <c r="E116" s="305">
-        <v>0.5</v>
+      <c r="E116" s="373">
+        <v>0.25</v>
       </c>
       <c r="F116" s="309">
         <v>0.5</v>
@@ -6957,6 +6984,9 @@
       <c r="C122" s="200"/>
       <c r="D122" t="s">
         <v>351</v>
+      </c>
+      <c r="H122" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="124" spans="1:13">
@@ -7066,10 +7096,10 @@
       <c r="A134" s="344" t="s">
         <v>404</v>
       </c>
-      <c r="B134" s="367" t="s">
+      <c r="B134" s="354" t="s">
         <v>405</v>
       </c>
-      <c r="C134" s="367"/>
+      <c r="C134" s="355"/>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="345">
@@ -7110,9 +7140,39 @@
         <v>407</v>
       </c>
     </row>
+    <row r="139" spans="1:5" ht="12" thickBot="1"/>
+    <row r="140" spans="1:5" ht="12" thickBot="1">
+      <c r="A140" s="356" t="s">
+        <v>408</v>
+      </c>
+      <c r="B140" s="357"/>
+      <c r="C140" s="358"/>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" s="93" t="s">
+        <v>35</v>
+      </c>
+      <c r="B141" s="94" t="s">
+        <v>37</v>
+      </c>
+      <c r="C141" s="95" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="12" thickBot="1">
+      <c r="A142" s="264">
+        <v>0.03</v>
+      </c>
+      <c r="B142" s="265">
+        <v>0.03</v>
+      </c>
+      <c r="C142" s="266">
+        <v>0.03</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="A140:C140"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="C1:H1"/>
@@ -7130,303 +7190,358 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.75">
-      <c r="A1" s="353" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="353" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="353" t="s">
-        <v>364</v>
-      </c>
-      <c r="D1" s="353" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" s="353" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="353" t="s">
-        <v>408</v>
-      </c>
-      <c r="G1" s="353" t="s">
-        <v>409</v>
-      </c>
-      <c r="H1" s="353" t="s">
-        <v>89</v>
-      </c>
-      <c r="I1" s="354" t="s">
-        <v>324</v>
-      </c>
-      <c r="J1" s="353" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="12.75">
-      <c r="A2" s="355">
+    <row r="1" spans="1:10">
+      <c r="A1">
+        <f>'Main Page'!B13</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <f>'Main Page'!B47</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="str">
+        <f>'Main Page'!C135</f>
+        <v>cylinder</v>
+      </c>
+      <c r="B3" t="str">
+        <f>'Main Page'!C136</f>
+        <v>s818_2702.dat</v>
+      </c>
+      <c r="C3" t="str">
+        <f>'Main Page'!C137</f>
+        <v>s825_2102.dat</v>
+      </c>
+      <c r="D3" t="str">
+        <f>'Main Page'!C138</f>
+        <v>s826_1602.dat</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <f>'Main Page'!A142</f>
+        <v>0.03</v>
+      </c>
+      <c r="B4">
+        <f>'Main Page'!B142</f>
+        <v>0.03</v>
+      </c>
+      <c r="C4">
+        <f>'Main Page'!C142</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="12.75">
+      <c r="A5" s="353" t="str">
+        <f>'Main Page'!A114</f>
+        <v>Station</v>
+      </c>
+      <c r="B5" s="353" t="str">
+        <f>'Main Page'!H113</f>
+        <v>Unit Weight</v>
+      </c>
+      <c r="C5" s="353" t="str">
+        <f>'Main Page'!B125</f>
+        <v>Twist</v>
+      </c>
+      <c r="D5" s="353" t="str">
+        <f>'Main Page'!L113</f>
+        <v>GJ</v>
+      </c>
+      <c r="E5" s="353" t="str">
+        <f>'Main Page'!K113</f>
+        <v>EA</v>
+      </c>
+      <c r="F5" s="353" t="str">
+        <f>'Main Page'!J113</f>
+        <v>EIEdge</v>
+      </c>
+      <c r="G5" s="353" t="str">
+        <f>'Main Page'!I113</f>
+        <v>EIFlap</v>
+      </c>
+      <c r="H5" s="353" t="str">
+        <f>'Main Page'!B113</f>
+        <v>Chord</v>
+      </c>
+      <c r="I5" s="353" t="str">
+        <f>'Main Page'!E113</f>
+        <v>Gen. Axis Loc.</v>
+      </c>
+      <c r="J5" s="353" t="str">
+        <f>'Main Page'!A134</f>
+        <v>Airfoil ID</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="12.75">
+      <c r="A6" s="353">
         <f>'Main Page'!A115</f>
         <v>0.05</v>
       </c>
-      <c r="B2" s="355">
+      <c r="B6" s="353">
         <f>'Main Page'!H115</f>
         <v>1181.9474017501359</v>
       </c>
-      <c r="C2" s="355">
+      <c r="C6" s="353">
         <f>'Main Page'!B127 - 'Main Page'!B$132</f>
         <v>11.1</v>
       </c>
-      <c r="D2" s="356">
+      <c r="D6" s="353">
         <f>'Main Page'!L115</f>
         <v>815590611.695804</v>
       </c>
-      <c r="E2" s="356">
+      <c r="E6" s="353">
         <f>'Main Page'!K115</f>
         <v>10326627046.93685</v>
       </c>
-      <c r="F2" s="356">
+      <c r="F6" s="353">
         <f>'Main Page'!J115</f>
         <v>2362406058.2721553</v>
       </c>
-      <c r="G2" s="356">
+      <c r="G6" s="353">
         <f>'Main Page'!I115</f>
         <v>2362406058.2721553</v>
       </c>
-      <c r="H2" s="355">
+      <c r="H6" s="353">
         <f>'Main Page'!B115</f>
         <v>1.349657099314199</v>
       </c>
-      <c r="I2" s="355">
+      <c r="I6" s="353">
         <f>'Main Page'!E115</f>
-        <v>0.5</v>
-      </c>
-      <c r="J2" s="353">
+        <v>0.25</v>
+      </c>
+      <c r="J6" s="353">
         <f>'Main Page'!D127</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12.75">
-      <c r="A3" s="355">
+    <row r="7" spans="1:10" ht="12.75">
+      <c r="A7" s="353">
         <f>'Main Page'!A116</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="B3" s="355">
+      <c r="B7" s="353">
         <f>'Main Page'!H116</f>
         <v>89.215305458599687</v>
       </c>
-      <c r="C3" s="355">
+      <c r="C7" s="353">
         <f>'Main Page'!B128 - 'Main Page'!B$132</f>
         <v>11.1</v>
       </c>
-      <c r="D3" s="356">
+      <c r="D7" s="353">
         <f>'Main Page'!L116</f>
         <v>102340392.98761402</v>
       </c>
-      <c r="E3" s="356">
+      <c r="E7" s="353">
         <f>'Main Page'!K116</f>
         <v>1295783621.589889</v>
       </c>
-      <c r="F3" s="356">
+      <c r="F7" s="353">
         <f>'Main Page'!J116</f>
         <v>292871613.66241747</v>
       </c>
-      <c r="G3" s="356">
+      <c r="G7" s="353">
         <f>'Main Page'!I116</f>
         <v>292871613.66241747</v>
       </c>
-      <c r="H3" s="355">
+      <c r="H7" s="353">
         <f>'Main Page'!B116</f>
         <v>1.3496570993141985</v>
       </c>
-      <c r="I3" s="355">
+      <c r="I7" s="353">
         <f>'Main Page'!E116</f>
-        <v>0.5</v>
-      </c>
-      <c r="J3" s="353">
+        <v>0.25</v>
+      </c>
+      <c r="J7" s="353">
         <f>'Main Page'!D128</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.75">
-      <c r="A4" s="355">
+    <row r="8" spans="1:10" ht="12.75">
+      <c r="A8" s="353">
         <f>'Main Page'!A117</f>
         <v>0.25</v>
       </c>
-      <c r="B4" s="355">
+      <c r="B8" s="353">
         <f>'Main Page'!H117</f>
         <v>117.20845675339662</v>
       </c>
-      <c r="C4" s="355">
+      <c r="C8" s="353">
         <f>'Main Page'!B129 - 'Main Page'!B$132</f>
         <v>11.1</v>
       </c>
-      <c r="D4" s="356">
+      <c r="D8" s="353">
         <f>'Main Page'!L117</f>
         <v>6059831.2604694702</v>
       </c>
-      <c r="E4" s="356">
+      <c r="E8" s="353">
         <f>'Main Page'!K117</f>
         <v>1535809947.6467729</v>
       </c>
-      <c r="F4" s="356">
+      <c r="F8" s="353">
         <f>'Main Page'!J117</f>
         <v>192688198.09657151</v>
       </c>
-      <c r="G4" s="356">
+      <c r="G8" s="353">
         <f>'Main Page'!I117</f>
         <v>71200412.886402056</v>
       </c>
-      <c r="H4" s="355">
+      <c r="H8" s="353">
         <f>'Main Page'!B117</f>
         <v>2</v>
       </c>
-      <c r="I4" s="355">
+      <c r="I8" s="353">
         <f>'Main Page'!E117</f>
         <v>0.34</v>
       </c>
-      <c r="J4" s="353">
+      <c r="J8" s="353">
         <f>'Main Page'!D129</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12.75">
-      <c r="A5" s="355">
+    <row r="9" spans="1:10" ht="12.75">
+      <c r="A9" s="353">
         <f>'Main Page'!A118</f>
         <v>0.5</v>
       </c>
-      <c r="B5" s="355">
+      <c r="B9" s="353">
         <f>'Main Page'!H118</f>
         <v>82.955569360022096</v>
       </c>
-      <c r="C5" s="355">
+      <c r="C9" s="353">
         <f>'Main Page'!B130 - 'Main Page'!B$132</f>
         <v>3.1</v>
       </c>
-      <c r="D5" s="356">
+      <c r="D9" s="353">
         <f>'Main Page'!L118</f>
         <v>2885752.229026631</v>
       </c>
-      <c r="E5" s="356">
+      <c r="E9" s="353">
         <f>'Main Page'!K118</f>
         <v>1094705409.6217237</v>
       </c>
-      <c r="F5" s="356">
+      <c r="F9" s="353">
         <f>'Main Page'!J118</f>
         <v>79116868.754064709</v>
       </c>
-      <c r="G5" s="356">
+      <c r="G9" s="353">
         <f>'Main Page'!I118</f>
         <v>22286831.062062379</v>
       </c>
-      <c r="H5" s="355">
+      <c r="H9" s="353">
         <f>'Main Page'!B118</f>
         <v>1.5334010668021336</v>
       </c>
-      <c r="I5" s="355">
+      <c r="I9" s="353">
         <f>'Main Page'!E118</f>
         <v>0.31</v>
       </c>
-      <c r="J5" s="353">
+      <c r="J9" s="353">
         <f>'Main Page'!D130</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="12.75">
-      <c r="A6" s="355">
+    <row r="10" spans="1:10" ht="12.75">
+      <c r="A10" s="353">
         <f>'Main Page'!A119</f>
         <v>0.75</v>
       </c>
-      <c r="B6" s="355">
+      <c r="B10" s="353">
         <f>'Main Page'!H119</f>
         <v>39.129612072462692</v>
       </c>
-      <c r="C6" s="355">
+      <c r="C10" s="353">
         <f>'Main Page'!B131 - 'Main Page'!B$132</f>
         <v>0.6</v>
       </c>
-      <c r="D6" s="356">
+      <c r="D10" s="353">
         <f>'Main Page'!L119</f>
         <v>574933.04560629011</v>
       </c>
-      <c r="E6" s="356">
+      <c r="E10" s="353">
         <f>'Main Page'!K119</f>
         <v>499093273.18287331</v>
       </c>
-      <c r="F6" s="356">
+      <c r="F10" s="353">
         <f>'Main Page'!J119</f>
         <v>21323059.849604025</v>
       </c>
-      <c r="G6" s="356">
+      <c r="G10" s="353">
         <f>'Main Page'!I119</f>
         <v>3549221.9475047868</v>
       </c>
-      <c r="H6" s="355">
+      <c r="H10" s="353">
         <f>'Main Page'!B119</f>
         <v>1.0670561341122682</v>
       </c>
-      <c r="I6" s="355">
+      <c r="I10" s="353">
         <f>'Main Page'!E119</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="J6" s="353">
+      <c r="J10" s="353">
         <f>'Main Page'!D131</f>
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="12.75">
-      <c r="A7" s="355">
+    <row r="11" spans="1:10" ht="12.75">
+      <c r="A11" s="353">
         <f>'Main Page'!A120</f>
         <v>1</v>
       </c>
-      <c r="B7" s="355">
+      <c r="B11" s="353">
         <f>'Main Page'!H120</f>
         <v>7.751396294306554</v>
       </c>
-      <c r="C7" s="355">
+      <c r="C11" s="353">
         <f>'Main Page'!B132 - 'Main Page'!B$132</f>
         <v>0</v>
       </c>
-      <c r="D7" s="356">
+      <c r="D11" s="353">
         <f>'Main Page'!L120</f>
         <v>61146.36439630347</v>
       </c>
-      <c r="E7" s="356">
+      <c r="E11" s="353">
         <f>'Main Page'!K120</f>
         <v>80734393.082686871</v>
       </c>
-      <c r="F7" s="356">
+      <c r="F11" s="353">
         <f>'Main Page'!J120</f>
         <v>2702250.8204062055</v>
       </c>
-      <c r="G7" s="356">
+      <c r="G11" s="353">
         <f>'Main Page'!I120</f>
         <v>79811.599091411103</v>
       </c>
-      <c r="H7" s="355">
+      <c r="H11" s="353">
         <f>'Main Page'!B120</f>
         <v>0.64719329438658879</v>
       </c>
-      <c r="I7" s="355">
+      <c r="I11" s="353">
         <f>'Main Page'!E120</f>
         <v>0.25</v>
       </c>
-      <c r="J7" s="353">
+      <c r="J11" s="353">
         <f>'Main Page'!D132</f>
         <v>4</v>
       </c>
@@ -7437,6 +7552,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <f>'Main Page'!B77</f>
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -7467,12 +7601,12 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="12" thickBot="1">
-      <c r="A2" s="368" t="s">
+      <c r="A2" s="369" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="369"/>
-      <c r="C2" s="369"/>
-      <c r="D2" s="370"/>
+      <c r="B2" s="370"/>
+      <c r="C2" s="370"/>
+      <c r="D2" s="371"/>
       <c r="F2" s="79" t="s">
         <v>54</v>
       </c>
@@ -8227,7 +8361,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -8235,7 +8369,7 @@
   <dimension ref="A1:T85"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D2" sqref="D2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -8272,11 +8406,11 @@
         <f>GECbladedata!D12-B3</f>
         <v>23.75</v>
       </c>
-      <c r="D2" s="371" t="s">
+      <c r="D2" s="356" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="372"/>
-      <c r="F2" s="373"/>
+      <c r="E2" s="357"/>
+      <c r="F2" s="358"/>
     </row>
     <row r="3" spans="1:20" ht="23.25" thickBot="1">
       <c r="A3" s="98" t="s">
@@ -8460,7 +8594,7 @@
       </c>
       <c r="G10" s="106">
         <f>GECbladedata!H28</f>
-        <v>0</v>
+        <v>0.33741427482854974</v>
       </c>
       <c r="H10" s="65">
         <f>GECbladedata!I28</f>
@@ -8468,7 +8602,7 @@
       </c>
       <c r="I10" s="106">
         <f>GECbladedata!J28</f>
-        <v>0</v>
+        <v>0.33741427482854974</v>
       </c>
       <c r="J10" s="105">
         <f>GECbladedata!K28</f>
@@ -8535,7 +8669,7 @@
       </c>
       <c r="G11" s="106">
         <f>GECbladedata!H29</f>
-        <v>0</v>
+        <v>0.33741427482854963</v>
       </c>
       <c r="H11" s="65">
         <f>GECbladedata!I29</f>
@@ -8543,7 +8677,7 @@
       </c>
       <c r="I11" s="106">
         <f>GECbladedata!J29</f>
-        <v>0</v>
+        <v>0.33741427482854963</v>
       </c>
       <c r="J11" s="105">
         <f>GECbladedata!K29</f>
@@ -8610,7 +8744,7 @@
       </c>
       <c r="G12" s="106">
         <f>GECbladedata!H30</f>
-        <v>1.4771354983247496E-2</v>
+        <v>0.29594991734037218</v>
       </c>
       <c r="H12" s="65">
         <f>GECbladedata!I30</f>
@@ -8618,7 +8752,7 @@
       </c>
       <c r="I12" s="106">
         <f>GECbladedata!J30</f>
-        <v>-5.6555553178479854E-3</v>
+        <v>0.27552300703927668</v>
       </c>
       <c r="J12" s="105">
         <f>GECbladedata!K30</f>
@@ -8685,7 +8819,7 @@
       </c>
       <c r="G13" s="106">
         <f>GECbladedata!H31</f>
-        <v>3.9390279955326658E-2</v>
+        <v>0.22684265486007649</v>
       </c>
       <c r="H13" s="65">
         <f>GECbladedata!I31</f>
@@ -8693,7 +8827,7 @@
       </c>
       <c r="I13" s="106">
         <f>GECbladedata!J31</f>
-        <v>-1.5081480847594629E-2</v>
+        <v>0.17237089405715517</v>
       </c>
       <c r="J13" s="105">
         <f>GECbladedata!K31</f>
@@ -8760,7 +8894,7 @@
       </c>
       <c r="G14" s="106">
         <f>GECbladedata!H32</f>
-        <v>6.4009204927405833E-2</v>
+        <v>0.15773539237978068</v>
       </c>
       <c r="H14" s="65">
         <f>GECbladedata!I32</f>
@@ -8768,7 +8902,7 @@
       </c>
       <c r="I14" s="106">
         <f>GECbladedata!J32</f>
-        <v>-2.4507406377341275E-2</v>
+        <v>6.9218781075033597E-2</v>
       </c>
       <c r="J14" s="105">
         <f>GECbladedata!K32</f>
@@ -10441,7 +10575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -10449,7 +10583,7 @@
   <dimension ref="B2:U50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -10579,7 +10713,7 @@
       </c>
       <c r="F5" s="204">
         <f>'Main Page'!E115</f>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G5" s="202">
         <f>'Main Page'!F115</f>
@@ -10613,6 +10747,7 @@
         <f>'Main Page'!M115</f>
         <v>538.24909552528584</v>
       </c>
+      <c r="P5" s="104"/>
     </row>
     <row r="6" spans="2:21">
       <c r="B6" s="208">
@@ -10633,7 +10768,7 @@
       </c>
       <c r="F6" s="204">
         <f>'Main Page'!E116</f>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G6" s="209">
         <f>'Main Page'!F116</f>
@@ -10667,6 +10802,7 @@
         <f>'Main Page'!M116</f>
         <v>40.627914067071856</v>
       </c>
+      <c r="P6" s="104"/>
     </row>
     <row r="7" spans="2:21">
       <c r="B7" s="198">
@@ -10721,6 +10857,7 @@
         <f>'Main Page'!M117</f>
         <v>24.149591455091301</v>
       </c>
+      <c r="P7" s="104"/>
     </row>
     <row r="8" spans="2:21">
       <c r="B8" s="198">
@@ -10775,6 +10912,7 @@
         <f>'Main Page'!M118</f>
         <v>9.0573611452431102</v>
       </c>
+      <c r="P8" s="104"/>
     </row>
     <row r="9" spans="2:21">
       <c r="B9" s="198">
@@ -10829,6 +10967,7 @@
         <f>'Main Page'!M119</f>
         <v>2.2054187533799334</v>
       </c>
+      <c r="P9" s="104"/>
     </row>
     <row r="10" spans="2:21">
       <c r="B10" s="216">
@@ -10883,6 +11022,7 @@
         <f>'Main Page'!M120</f>
         <v>0.25688857997871806</v>
       </c>
+      <c r="P10" s="104"/>
     </row>
     <row r="11" spans="2:21">
       <c r="J11" s="102"/>
@@ -11102,14 +11242,14 @@
       </c>
       <c r="H18" s="228">
         <f t="shared" ref="H18:H23" si="4">C5*(G5-F5)</f>
-        <v>0</v>
+        <v>0.33741427482854974</v>
       </c>
       <c r="I18" s="186">
         <v>0</v>
       </c>
       <c r="J18" s="240">
         <f t="shared" ref="J18:J23" si="5">C5*(H5-F5)</f>
-        <v>0</v>
+        <v>0.33741427482854974</v>
       </c>
       <c r="K18" s="239">
         <f>'Main Page'!B127-'Main Page'!B$132</f>
@@ -11172,14 +11312,14 @@
       </c>
       <c r="H19" s="245">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.33741427482854963</v>
       </c>
       <c r="I19" s="8">
         <v>0</v>
       </c>
       <c r="J19" s="246">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.33741427482854963</v>
       </c>
       <c r="K19" s="244">
         <f>'Main Page'!B128-'Main Page'!B$132</f>
@@ -11637,7 +11777,7 @@
       </c>
       <c r="H28" s="228">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.33741427482854974</v>
       </c>
       <c r="I28" s="186">
         <f t="shared" si="11"/>
@@ -11645,7 +11785,7 @@
       </c>
       <c r="J28" s="240">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.33741427482854974</v>
       </c>
       <c r="K28" s="239">
         <f t="shared" si="11"/>
@@ -11711,7 +11851,7 @@
       </c>
       <c r="H29" s="245">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>0.33741427482854963</v>
       </c>
       <c r="I29" s="8">
         <f t="shared" si="12"/>
@@ -11719,7 +11859,7 @@
       </c>
       <c r="J29" s="246">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>0.33741427482854963</v>
       </c>
       <c r="K29" s="244">
         <f t="shared" si="12"/>
@@ -11784,7 +11924,7 @@
       </c>
       <c r="H30" s="245">
         <f>H$29+($B30-$B$29)*(H$33-H$29)/($B$33-$B$29)</f>
-        <v>1.4771354983247496E-2</v>
+        <v>0.29594991734037218</v>
       </c>
       <c r="I30" s="8">
         <f t="shared" ref="I30:Q32" si="13">I$29+($B30-$B$29)*(I$33-I$29)/($B$33-$B$29)</f>
@@ -11792,7 +11932,7 @@
       </c>
       <c r="J30" s="246">
         <f t="shared" si="13"/>
-        <v>-5.6555553178479854E-3</v>
+        <v>0.27552300703927668</v>
       </c>
       <c r="K30" s="244">
         <f t="shared" si="13"/>
@@ -11857,7 +11997,7 @@
       </c>
       <c r="H31" s="245">
         <f t="shared" si="16"/>
-        <v>3.9390279955326658E-2</v>
+        <v>0.22684265486007649</v>
       </c>
       <c r="I31" s="8">
         <f t="shared" si="13"/>
@@ -11865,7 +12005,7 @@
       </c>
       <c r="J31" s="246">
         <f t="shared" si="13"/>
-        <v>-1.5081480847594629E-2</v>
+        <v>0.17237089405715517</v>
       </c>
       <c r="K31" s="244">
         <f t="shared" si="13"/>
@@ -11930,7 +12070,7 @@
       </c>
       <c r="H32" s="245">
         <f t="shared" si="16"/>
-        <v>6.4009204927405833E-2</v>
+        <v>0.15773539237978068</v>
       </c>
       <c r="I32" s="8">
         <f t="shared" si="13"/>
@@ -11938,7 +12078,7 @@
       </c>
       <c r="J32" s="246">
         <f t="shared" si="13"/>
-        <v>-2.4507406377341275E-2</v>
+        <v>6.9218781075033597E-2</v>
       </c>
       <c r="K32" s="244">
         <f t="shared" si="13"/>
@@ -13160,7 +13300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O26"/>
   <sheetViews>
@@ -13986,14 +14126,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Y131"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="75" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -14942,12 +15082,12 @@
       <c r="A19" s="113"/>
       <c r="B19" s="166"/>
       <c r="C19" s="113"/>
-      <c r="D19" s="374" t="s">
+      <c r="D19" s="372" t="s">
         <v>240</v>
       </c>
-      <c r="E19" s="374"/>
-      <c r="F19" s="374"/>
-      <c r="G19" s="374"/>
+      <c r="E19" s="372"/>
+      <c r="F19" s="372"/>
+      <c r="G19" s="372"/>
       <c r="H19" s="113"/>
       <c r="I19" s="113"/>
       <c r="J19" s="122"/>

</xml_diff>

<commit_message>
Another FAST file ``backup'', so to speak
</commit_message>
<xml_diff>
--- a/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
+++ b/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="411">
   <si>
     <t>number</t>
   </si>
@@ -1724,6 +1724,9 @@
   </si>
   <si>
     <t>Cylinder changed to produce correct AeroCent</t>
+  </si>
+  <si>
+    <t>&lt;---- switched order to flap, flap, edge</t>
   </si>
 </sst>
 </file>
@@ -2587,7 +2590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="374">
+  <cellXfs count="380">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3388,6 +3391,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="19" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3433,7 +3439,20 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4017,11 +4036,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="82432768"/>
-        <c:axId val="82434688"/>
+        <c:axId val="99322112"/>
+        <c:axId val="99341056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82432768"/>
+        <c:axId val="99322112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4106,12 +4125,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82434688"/>
+        <c:crossAx val="99341056"/>
         <c:crossesAt val="-10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82434688"/>
+        <c:axId val="99341056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4195,7 +4214,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82432768"/>
+        <c:crossAx val="99322112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4757,6 +4776,18 @@
             </a:rPr>
             <a:t>                          Changed AC for cylinders to yield correct AeroCent</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	Switched modal damping order</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1000">
             <a:effectLst/>
           </a:endParaRPr>
@@ -5254,10 +5285,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U142"/>
+  <dimension ref="A1:U149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H123" sqref="H123"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T62" sqref="T62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -5281,14 +5312,14 @@
       <c r="B1" s="337" t="s">
         <v>401</v>
       </c>
-      <c r="C1" s="365" t="s">
+      <c r="C1" s="366" t="s">
         <v>402</v>
       </c>
-      <c r="D1" s="366"/>
-      <c r="E1" s="366"/>
-      <c r="F1" s="366"/>
-      <c r="G1" s="366"/>
-      <c r="H1" s="367"/>
+      <c r="D1" s="367"/>
+      <c r="E1" s="367"/>
+      <c r="F1" s="367"/>
+      <c r="G1" s="367"/>
+      <c r="H1" s="368"/>
     </row>
     <row r="2" spans="1:8" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="A2" s="60" t="s">
@@ -5304,17 +5335,17 @@
       <c r="A3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="359" t="s">
+      <c r="B3" s="360" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="360"/>
-      <c r="D3" s="361"/>
+      <c r="C3" s="361"/>
+      <c r="D3" s="362"/>
       <c r="E3" s="35"/>
-      <c r="F3" s="362" t="s">
+      <c r="F3" s="363" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="363"/>
-      <c r="H3" s="364"/>
+      <c r="G3" s="364"/>
+      <c r="H3" s="365"/>
     </row>
     <row r="4" spans="1:8" ht="12" thickBot="1">
       <c r="A4" s="20" t="s">
@@ -5577,11 +5608,11 @@
       <c r="C18" s="330">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D18" s="368" t="s">
+      <c r="D18" s="369" t="s">
         <v>374</v>
       </c>
-      <c r="E18" s="367"/>
-      <c r="F18" s="367"/>
+      <c r="E18" s="368"/>
+      <c r="F18" s="368"/>
     </row>
     <row r="19" spans="1:21" ht="25.5" customHeight="1">
       <c r="A19" s="267" t="s">
@@ -5593,11 +5624,11 @@
       <c r="C19" s="330">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D19" s="368" t="s">
+      <c r="D19" s="369" t="s">
         <v>373</v>
       </c>
-      <c r="E19" s="367"/>
-      <c r="F19" s="367"/>
+      <c r="E19" s="368"/>
+      <c r="F19" s="368"/>
       <c r="I19" s="35" t="s">
         <v>69</v>
       </c>
@@ -6744,7 +6775,7 @@
       <c r="D115" s="304" t="s">
         <v>378</v>
       </c>
-      <c r="E115" s="373">
+      <c r="E115" s="356">
         <v>0.25</v>
       </c>
       <c r="F115" s="303">
@@ -6785,7 +6816,7 @@
       <c r="D116" s="310" t="s">
         <v>378</v>
       </c>
-      <c r="E116" s="373">
+      <c r="E116" s="356">
         <v>0.25</v>
       </c>
       <c r="F116" s="309">
@@ -7142,33 +7173,66 @@
     </row>
     <row r="139" spans="1:5" ht="12" thickBot="1"/>
     <row r="140" spans="1:5" ht="12" thickBot="1">
-      <c r="A140" s="356" t="s">
+      <c r="A140" s="357" t="s">
         <v>408</v>
       </c>
-      <c r="B140" s="357"/>
-      <c r="C140" s="358"/>
+      <c r="B140" s="358"/>
+      <c r="C140" s="359"/>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="B141" s="94" t="s">
+      <c r="B141" s="375" t="s">
+        <v>36</v>
+      </c>
+      <c r="C141" s="374" t="s">
         <v>37</v>
       </c>
-      <c r="C141" s="95" t="s">
-        <v>36</v>
+      <c r="E141" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="12" thickBot="1">
       <c r="A142" s="264">
         <v>0.03</v>
       </c>
-      <c r="B142" s="265">
+      <c r="B142" s="376">
         <v>0.03</v>
       </c>
-      <c r="C142" s="266">
+      <c r="C142" s="377">
         <v>0.03</v>
       </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="5"/>
+      <c r="B145" s="378"/>
+      <c r="C145" s="378"/>
+      <c r="D145" s="378"/>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="5"/>
+      <c r="B146" s="378"/>
+      <c r="C146" s="378"/>
+      <c r="D146" s="378"/>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="5"/>
+      <c r="B147" s="378"/>
+      <c r="C147" s="379"/>
+      <c r="D147" s="378"/>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="5"/>
+      <c r="B148" s="378"/>
+      <c r="C148" s="378"/>
+      <c r="D148" s="378"/>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="5"/>
+      <c r="B149" s="378"/>
+      <c r="C149" s="378"/>
+      <c r="D149" s="378"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -7193,7 +7257,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -7601,12 +7665,12 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="12" thickBot="1">
-      <c r="A2" s="369" t="s">
+      <c r="A2" s="370" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="370"/>
-      <c r="C2" s="370"/>
-      <c r="D2" s="371"/>
+      <c r="B2" s="371"/>
+      <c r="C2" s="371"/>
+      <c r="D2" s="372"/>
       <c r="F2" s="79" t="s">
         <v>54</v>
       </c>
@@ -8406,11 +8470,11 @@
         <f>GECbladedata!D12-B3</f>
         <v>23.75</v>
       </c>
-      <c r="D2" s="356" t="s">
+      <c r="D2" s="357" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="357"/>
-      <c r="F2" s="358"/>
+      <c r="E2" s="358"/>
+      <c r="F2" s="359"/>
     </row>
     <row r="3" spans="1:20" ht="23.25" thickBot="1">
       <c r="A3" s="98" t="s">
@@ -15082,12 +15146,12 @@
       <c r="A19" s="113"/>
       <c r="B19" s="166"/>
       <c r="C19" s="113"/>
-      <c r="D19" s="372" t="s">
+      <c r="D19" s="373" t="s">
         <v>240</v>
       </c>
-      <c r="E19" s="372"/>
-      <c r="F19" s="372"/>
-      <c r="G19" s="372"/>
+      <c r="E19" s="373"/>
+      <c r="F19" s="373"/>
+      <c r="G19" s="373"/>
       <c r="H19" s="113"/>
       <c r="I19" s="113"/>
       <c r="J19" s="122"/>

</xml_diff>

<commit_message>
WindPACT plus general FAST utility
Code to generate turbine dictionary, create FAST file templates,
create FAST input files, load FAST, and much more!
</commit_message>
<xml_diff>
--- a/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
+++ b/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
@@ -3394,6 +3394,22 @@
     <xf numFmtId="164" fontId="19" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3437,22 +3453,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4036,11 +4036,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="99322112"/>
-        <c:axId val="99341056"/>
+        <c:axId val="100789632"/>
+        <c:axId val="114582656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99322112"/>
+        <c:axId val="100789632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4125,12 +4125,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99341056"/>
+        <c:crossAx val="114582656"/>
         <c:crossesAt val="-10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99341056"/>
+        <c:axId val="114582656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4214,7 +4214,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99322112"/>
+        <c:crossAx val="100789632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5287,8 +5287,8 @@
   </sheetPr>
   <dimension ref="A1:U149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T62" sqref="T62"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -5312,14 +5312,14 @@
       <c r="B1" s="337" t="s">
         <v>401</v>
       </c>
-      <c r="C1" s="366" t="s">
+      <c r="C1" s="372" t="s">
         <v>402</v>
       </c>
-      <c r="D1" s="367"/>
-      <c r="E1" s="367"/>
-      <c r="F1" s="367"/>
-      <c r="G1" s="367"/>
-      <c r="H1" s="368"/>
+      <c r="D1" s="373"/>
+      <c r="E1" s="373"/>
+      <c r="F1" s="373"/>
+      <c r="G1" s="373"/>
+      <c r="H1" s="374"/>
     </row>
     <row r="2" spans="1:8" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="A2" s="60" t="s">
@@ -5335,17 +5335,17 @@
       <c r="A3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="360" t="s">
+      <c r="B3" s="366" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="361"/>
-      <c r="D3" s="362"/>
+      <c r="C3" s="367"/>
+      <c r="D3" s="368"/>
       <c r="E3" s="35"/>
-      <c r="F3" s="363" t="s">
+      <c r="F3" s="369" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="364"/>
-      <c r="H3" s="365"/>
+      <c r="G3" s="370"/>
+      <c r="H3" s="371"/>
     </row>
     <row r="4" spans="1:8" ht="12" thickBot="1">
       <c r="A4" s="20" t="s">
@@ -5553,8 +5553,8 @@
         <v>43</v>
       </c>
       <c r="B14" s="336">
-        <f>PI()*(B58^4-B59^4)/2/(GECdrivetrain!C7)*GECtwrdata!F7</f>
-        <v>2074343118.9103956</v>
+        <f>PI()*(B58^4-B59^4)/32/(GECdrivetrain!C7)*GECtwrdata!F7</f>
+        <v>129646444.93189973</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="22.5">
@@ -5608,11 +5608,11 @@
       <c r="C18" s="330">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D18" s="369" t="s">
+      <c r="D18" s="375" t="s">
         <v>374</v>
       </c>
-      <c r="E18" s="368"/>
-      <c r="F18" s="368"/>
+      <c r="E18" s="374"/>
+      <c r="F18" s="374"/>
     </row>
     <row r="19" spans="1:21" ht="25.5" customHeight="1">
       <c r="A19" s="267" t="s">
@@ -5624,11 +5624,11 @@
       <c r="C19" s="330">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D19" s="369" t="s">
+      <c r="D19" s="375" t="s">
         <v>373</v>
       </c>
-      <c r="E19" s="368"/>
-      <c r="F19" s="368"/>
+      <c r="E19" s="374"/>
+      <c r="F19" s="374"/>
       <c r="I19" s="35" t="s">
         <v>69</v>
       </c>
@@ -7173,20 +7173,20 @@
     </row>
     <row r="139" spans="1:5" ht="12" thickBot="1"/>
     <row r="140" spans="1:5" ht="12" thickBot="1">
-      <c r="A140" s="357" t="s">
+      <c r="A140" s="363" t="s">
         <v>408</v>
       </c>
-      <c r="B140" s="358"/>
-      <c r="C140" s="359"/>
+      <c r="B140" s="364"/>
+      <c r="C140" s="365"/>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="B141" s="375" t="s">
+      <c r="B141" s="358" t="s">
         <v>36</v>
       </c>
-      <c r="C141" s="374" t="s">
+      <c r="C141" s="357" t="s">
         <v>37</v>
       </c>
       <c r="E141" t="s">
@@ -7197,42 +7197,42 @@
       <c r="A142" s="264">
         <v>0.03</v>
       </c>
-      <c r="B142" s="376">
+      <c r="B142" s="359">
         <v>0.03</v>
       </c>
-      <c r="C142" s="377">
+      <c r="C142" s="360">
         <v>0.03</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="5"/>
-      <c r="B145" s="378"/>
-      <c r="C145" s="378"/>
-      <c r="D145" s="378"/>
+      <c r="B145" s="361"/>
+      <c r="C145" s="361"/>
+      <c r="D145" s="361"/>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="5"/>
-      <c r="B146" s="378"/>
-      <c r="C146" s="378"/>
-      <c r="D146" s="378"/>
+      <c r="B146" s="361"/>
+      <c r="C146" s="361"/>
+      <c r="D146" s="361"/>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="5"/>
-      <c r="B147" s="378"/>
-      <c r="C147" s="379"/>
-      <c r="D147" s="378"/>
+      <c r="B147" s="361"/>
+      <c r="C147" s="362"/>
+      <c r="D147" s="361"/>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="5"/>
-      <c r="B148" s="378"/>
-      <c r="C148" s="378"/>
-      <c r="D148" s="378"/>
+      <c r="B148" s="361"/>
+      <c r="C148" s="361"/>
+      <c r="D148" s="361"/>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="5"/>
-      <c r="B149" s="378"/>
-      <c r="C149" s="378"/>
-      <c r="D149" s="378"/>
+      <c r="B149" s="361"/>
+      <c r="C149" s="361"/>
+      <c r="D149" s="361"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -7665,12 +7665,12 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="12" thickBot="1">
-      <c r="A2" s="370" t="s">
+      <c r="A2" s="376" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="371"/>
-      <c r="C2" s="371"/>
-      <c r="D2" s="372"/>
+      <c r="B2" s="377"/>
+      <c r="C2" s="377"/>
+      <c r="D2" s="378"/>
       <c r="F2" s="79" t="s">
         <v>54</v>
       </c>
@@ -8470,11 +8470,11 @@
         <f>GECbladedata!D12-B3</f>
         <v>23.75</v>
       </c>
-      <c r="D2" s="357" t="s">
+      <c r="D2" s="363" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="358"/>
-      <c r="F2" s="359"/>
+      <c r="E2" s="364"/>
+      <c r="F2" s="365"/>
     </row>
     <row r="3" spans="1:20" ht="23.25" thickBot="1">
       <c r="A3" s="98" t="s">
@@ -15146,12 +15146,12 @@
       <c r="A19" s="113"/>
       <c r="B19" s="166"/>
       <c r="C19" s="113"/>
-      <c r="D19" s="373" t="s">
+      <c r="D19" s="379" t="s">
         <v>240</v>
       </c>
-      <c r="E19" s="373"/>
-      <c r="F19" s="373"/>
-      <c r="G19" s="373"/>
+      <c r="E19" s="379"/>
+      <c r="F19" s="379"/>
+      <c r="G19" s="379"/>
       <c r="H19" s="113"/>
       <c r="I19" s="113"/>
       <c r="J19" s="122"/>

</xml_diff>

<commit_message>
Debugging freaking FAST models and their stupid instabilities
</commit_message>
<xml_diff>
--- a/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
+++ b/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="705" windowWidth="17565" windowHeight="12990" activeTab="2"/>
+    <workbookView xWindow="1560" yWindow="705" windowWidth="17565" windowHeight="12990"/>
   </bookViews>
   <sheets>
     <sheet name="Main Page" sheetId="5" r:id="rId1"/>
@@ -4292,11 +4292,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="82863616"/>
-        <c:axId val="82865536"/>
+        <c:axId val="75985664"/>
+        <c:axId val="75987584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82863616"/>
+        <c:axId val="75985664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4381,12 +4381,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82865536"/>
+        <c:crossAx val="75987584"/>
         <c:crossesAt val="-10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82865536"/>
+        <c:axId val="75987584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4470,7 +4470,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82863616"/>
+        <c:crossAx val="75985664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5543,8 +5543,8 @@
   </sheetPr>
   <dimension ref="A1:U155"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -8427,7 +8427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updating parameters with new pitch control actuator
</commit_message>
<xml_diff>
--- a/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
+++ b/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrinker\Documents\GitHub\dissertation\FAST_models\WindPACT\excel_proc\turbines\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="710" windowWidth="17570" windowHeight="12990" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="1560" yWindow="705" windowWidth="17565" windowHeight="12990" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Main Page" sheetId="5" r:id="rId1"/>
@@ -27,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="7">'Blade Data'!$A$6:$Q$32</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -37,7 +32,7 @@
     <author>Jeff Minnema</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="515">
   <si>
     <t>number</t>
   </si>
@@ -2035,6 +2030,18 @@
   </si>
   <si>
     <t>N-m</t>
+  </si>
+  <si>
+    <t>P2P_Num</t>
+  </si>
+  <si>
+    <t>P2P_Den</t>
+  </si>
+  <si>
+    <t>numerator blade pitch actuator TF</t>
+  </si>
+  <si>
+    <t>denominator blade pitch actuator TF</t>
   </si>
 </sst>
 </file>
@@ -4472,11 +4479,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="319611736"/>
-        <c:axId val="319616048"/>
+        <c:axId val="95175808"/>
+        <c:axId val="95177728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="319611736"/>
+        <c:axId val="95175808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4561,12 +4568,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319616048"/>
+        <c:crossAx val="95177728"/>
         <c:crossesAt val="-10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="319616048"/>
+        <c:axId val="95177728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4650,7 +4657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319611736"/>
+        <c:crossAx val="95175808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5730,19 +5737,19 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="8" width="12.109375" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" customWidth="1"/>
+    <col min="7" max="8" width="12.1640625" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="41.25" customHeight="1" thickBot="1">
@@ -5787,7 +5794,7 @@
       <c r="G3" s="403"/>
       <c r="H3" s="404"/>
     </row>
-    <row r="4" spans="1:8" ht="11" thickBot="1">
+    <row r="4" spans="1:8" ht="12" thickBot="1">
       <c r="A4" s="20" t="s">
         <v>5</v>
       </c>
@@ -5912,7 +5919,7 @@
         <v>1751.6710645266089</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="10.5" thickBot="1">
+    <row r="8" spans="1:8" ht="12" thickBot="1">
       <c r="A8" s="23" t="s">
         <v>12</v>
       </c>
@@ -5945,7 +5952,7 @@
         <v>7485.1732085651756</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="10.5" thickBot="1">
+    <row r="9" spans="1:8" ht="12" thickBot="1">
       <c r="A9" s="106" t="s">
         <v>120</v>
       </c>
@@ -5988,7 +5995,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="20">
+    <row r="14" spans="1:8" ht="22.5">
       <c r="A14" s="61" t="s">
         <v>43</v>
       </c>
@@ -6025,7 +6032,7 @@
       </c>
       <c r="E16" s="353"/>
     </row>
-    <row r="17" spans="1:21" ht="23.5" customHeight="1">
+    <row r="17" spans="1:21" ht="23.45" customHeight="1">
       <c r="A17" s="61" t="s">
         <v>42</v>
       </c>
@@ -6102,7 +6109,7 @@
       <c r="O20" s="170"/>
       <c r="P20" s="171"/>
     </row>
-    <row r="21" spans="1:21" ht="11.5" customHeight="1">
+    <row r="21" spans="1:21" ht="11.45" customHeight="1">
       <c r="A21" s="61" t="s">
         <v>31</v>
       </c>
@@ -6148,7 +6155,7 @@
       <c r="O23" s="8"/>
       <c r="P23" s="173"/>
     </row>
-    <row r="24" spans="1:21" ht="12.65" customHeight="1">
+    <row r="24" spans="1:21" ht="12.6" customHeight="1">
       <c r="A24" s="100" t="s">
         <v>74</v>
       </c>
@@ -6169,7 +6176,7 @@
       <c r="O24" s="8"/>
       <c r="P24" s="173"/>
     </row>
-    <row r="25" spans="1:21" ht="10.5" thickBot="1">
+    <row r="25" spans="1:21" ht="12" thickBot="1">
       <c r="A25" s="100" t="s">
         <v>75</v>
       </c>
@@ -6200,7 +6207,7 @@
       <c r="G26" s="89"/>
       <c r="H26" s="12"/>
     </row>
-    <row r="28" spans="1:21" ht="12.65" customHeight="1">
+    <row r="28" spans="1:21" ht="12.6" customHeight="1">
       <c r="A28" s="109" t="s">
         <v>78</v>
       </c>
@@ -6240,7 +6247,7 @@
     <row r="32" spans="1:21">
       <c r="B32" s="53"/>
     </row>
-    <row r="33" spans="1:5" ht="10.5">
+    <row r="33" spans="1:5">
       <c r="A33" s="109" t="s">
         <v>80</v>
       </c>
@@ -6413,7 +6420,7 @@
         <v>3.1469175392670157</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="10.5">
+    <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
         <v>12</v>
       </c>
@@ -6526,7 +6533,7 @@
       <c r="A64" s="18"/>
       <c r="B64" s="124"/>
     </row>
-    <row r="65" spans="1:4" ht="10.5">
+    <row r="65" spans="1:4">
       <c r="A65" s="111" t="s">
         <v>137</v>
       </c>
@@ -6611,7 +6618,7 @@
       <c r="A72" s="18"/>
       <c r="B72" s="124"/>
     </row>
-    <row r="73" spans="1:4" ht="10.5">
+    <row r="73" spans="1:4">
       <c r="A73" s="111" t="s">
         <v>143</v>
       </c>
@@ -6693,7 +6700,7 @@
       <c r="A80" s="18"/>
       <c r="B80" s="125"/>
     </row>
-    <row r="81" spans="1:4" ht="10.5">
+    <row r="81" spans="1:4">
       <c r="A81" s="111" t="s">
         <v>152</v>
       </c>
@@ -6793,7 +6800,7 @@
       <c r="A90" s="18"/>
       <c r="B90" s="123"/>
     </row>
-    <row r="91" spans="1:4" ht="10.5">
+    <row r="91" spans="1:4">
       <c r="A91" s="111" t="s">
         <v>158</v>
       </c>
@@ -6850,7 +6857,7 @@
       <c r="A96" s="18"/>
       <c r="B96" s="126"/>
     </row>
-    <row r="97" spans="1:4" ht="10.5">
+    <row r="97" spans="1:4">
       <c r="A97" s="111" t="s">
         <v>162</v>
       </c>
@@ -6964,7 +6971,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="10.5">
+    <row r="108" spans="1:4">
       <c r="A108" s="111" t="s">
         <v>387</v>
       </c>
@@ -7027,7 +7034,7 @@
       <c r="I113" s="183"/>
       <c r="J113" s="183"/>
     </row>
-    <row r="114" spans="1:13" ht="15">
+    <row r="114" spans="1:13" ht="14.25">
       <c r="A114" s="184"/>
       <c r="B114" s="185"/>
       <c r="C114" s="186" t="s">
@@ -7085,7 +7092,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="11.5">
+    <row r="116" spans="1:13" ht="12">
       <c r="A116" s="281">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -7120,7 +7127,7 @@
         <v>2.3240623855198695E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="11.5">
+    <row r="117" spans="1:13" ht="12">
       <c r="A117" s="290">
         <v>0.25</v>
       </c>
@@ -7155,7 +7162,7 @@
         <v>6.6795086790909508E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="11.5">
+    <row r="118" spans="1:13" ht="12">
       <c r="A118" s="290">
         <v>0.5</v>
       </c>
@@ -7190,7 +7197,7 @@
         <v>1.2515851111560431E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="11.5">
+    <row r="119" spans="1:13" ht="12">
       <c r="A119" s="293">
         <v>0.75</v>
       </c>
@@ -7556,7 +7563,7 @@
         <v>0.25688857997871806</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="13">
+    <row r="131" spans="1:13">
       <c r="B131" s="18" t="s">
         <v>349</v>
       </c>
@@ -7573,7 +7580,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="10.5">
+    <row r="134" spans="1:13">
       <c r="A134" s="184"/>
       <c r="B134" s="230" t="s">
         <v>363</v>
@@ -7583,7 +7590,7 @@
       </c>
       <c r="D134" s="392"/>
     </row>
-    <row r="135" spans="1:13" ht="11.5">
+    <row r="135" spans="1:13" ht="12">
       <c r="A135" s="192" t="s">
         <v>87</v>
       </c>
@@ -7671,7 +7678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="11.5">
+    <row r="143" spans="1:13" ht="12">
       <c r="A143" s="340" t="s">
         <v>399</v>
       </c>
@@ -7732,8 +7739,8 @@
       <c r="F147" s="353"/>
       <c r="G147" s="353"/>
     </row>
-    <row r="148" spans="1:7" ht="10.5" thickBot="1"/>
-    <row r="149" spans="1:7" ht="10.5" thickBot="1">
+    <row r="148" spans="1:7" ht="12" thickBot="1"/>
+    <row r="149" spans="1:7" ht="12" thickBot="1">
       <c r="A149" s="395" t="s">
         <v>401</v>
       </c>
@@ -7744,7 +7751,7 @@
       </c>
       <c r="F149" s="353"/>
     </row>
-    <row r="150" spans="1:7" ht="10.5" thickBot="1">
+    <row r="150" spans="1:7" ht="12" thickBot="1">
       <c r="A150" s="362" t="s">
         <v>35</v>
       </c>
@@ -7759,7 +7766,7 @@
       </c>
       <c r="F150" s="353"/>
     </row>
-    <row r="151" spans="1:7" ht="11" thickBot="1">
+    <row r="151" spans="1:7" ht="12" thickBot="1">
       <c r="A151" s="364">
         <v>3.882E-2</v>
       </c>
@@ -7774,8 +7781,8 @@
       </c>
       <c r="F151" s="353"/>
     </row>
-    <row r="152" spans="1:7" ht="10.5" thickBot="1"/>
-    <row r="153" spans="1:7" ht="10.5" thickBot="1">
+    <row r="152" spans="1:7" ht="12" thickBot="1"/>
+    <row r="153" spans="1:7" ht="12" thickBot="1">
       <c r="A153" s="395" t="s">
         <v>410</v>
       </c>
@@ -7786,7 +7793,7 @@
       </c>
       <c r="F153" s="353"/>
     </row>
-    <row r="154" spans="1:7" ht="10.5">
+    <row r="154" spans="1:7">
       <c r="A154" s="367" t="s">
         <v>50</v>
       </c>
@@ -7799,7 +7806,7 @@
       </c>
       <c r="F154" s="353"/>
     </row>
-    <row r="155" spans="1:7" ht="10.5">
+    <row r="155" spans="1:7">
       <c r="A155" s="369" t="s">
         <v>51</v>
       </c>
@@ -7812,7 +7819,7 @@
       </c>
       <c r="F155" s="353"/>
     </row>
-    <row r="156" spans="1:7" ht="10.5">
+    <row r="156" spans="1:7">
       <c r="A156" s="372" t="s">
         <v>52</v>
       </c>
@@ -7824,7 +7831,7 @@
       </c>
       <c r="F156" s="353"/>
     </row>
-    <row r="157" spans="1:7" ht="11" thickBot="1">
+    <row r="157" spans="1:7" ht="12" thickBot="1">
       <c r="A157" s="373" t="s">
         <v>53</v>
       </c>
@@ -7869,10 +7876,10 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -8738,23 +8745,23 @@
       <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="10" max="11" width="9.6640625" customWidth="1"/>
-    <col min="12" max="12" width="9.44140625" customWidth="1"/>
+    <col min="12" max="12" width="9.5" customWidth="1"/>
     <col min="13" max="14" width="11.33203125" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" customWidth="1"/>
+    <col min="15" max="15" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="12.5">
+    <row r="1" spans="1:25" ht="12.75">
       <c r="A1" s="112"/>
       <c r="B1" s="112" t="s">
         <v>170</v>
@@ -8786,7 +8793,7 @@
       <c r="X1" s="112"/>
       <c r="Y1" s="112"/>
     </row>
-    <row r="2" spans="1:25" ht="12.5">
+    <row r="2" spans="1:25" ht="12.75">
       <c r="A2" s="112"/>
       <c r="B2" s="113" t="s">
         <v>171</v>
@@ -8818,7 +8825,7 @@
       <c r="X2" s="112"/>
       <c r="Y2" s="112"/>
     </row>
-    <row r="3" spans="1:25" ht="12.5">
+    <row r="3" spans="1:25" ht="12.75">
       <c r="A3" s="112"/>
       <c r="B3" s="112"/>
       <c r="C3" s="112"/>
@@ -8845,7 +8852,7 @@
       <c r="X3" s="112"/>
       <c r="Y3" s="112"/>
     </row>
-    <row r="4" spans="1:25" ht="37.5">
+    <row r="4" spans="1:25" ht="38.25">
       <c r="A4" s="115"/>
       <c r="B4" s="163" t="s">
         <v>172</v>
@@ -8904,7 +8911,7 @@
       <c r="X4" s="115"/>
       <c r="Y4" s="116"/>
     </row>
-    <row r="5" spans="1:25" ht="12.5">
+    <row r="5" spans="1:25" ht="12.75">
       <c r="A5" s="112"/>
       <c r="B5" s="164" t="s">
         <v>12</v>
@@ -8974,7 +8981,7 @@
       <c r="X5" s="112"/>
       <c r="Y5" s="112"/>
     </row>
-    <row r="6" spans="1:25" ht="12.5">
+    <row r="6" spans="1:25" ht="12.75">
       <c r="A6" s="112"/>
       <c r="B6" s="164" t="s">
         <v>184</v>
@@ -9035,7 +9042,7 @@
       <c r="X6" s="112"/>
       <c r="Y6" s="112"/>
     </row>
-    <row r="7" spans="1:25" ht="12.5">
+    <row r="7" spans="1:25" ht="12.75">
       <c r="A7" s="112"/>
       <c r="B7" s="164" t="s">
         <v>137</v>
@@ -9108,7 +9115,7 @@
       <c r="X7" s="112"/>
       <c r="Y7" s="112"/>
     </row>
-    <row r="8" spans="1:25" ht="12.5">
+    <row r="8" spans="1:25" ht="12.75">
       <c r="A8" s="112"/>
       <c r="B8" s="164" t="s">
         <v>185</v>
@@ -9171,7 +9178,7 @@
       <c r="X8" s="112"/>
       <c r="Y8" s="118"/>
     </row>
-    <row r="9" spans="1:25" ht="12.5">
+    <row r="9" spans="1:25" ht="12.75">
       <c r="A9" s="112"/>
       <c r="B9" s="164" t="s">
         <v>186</v>
@@ -9234,7 +9241,7 @@
       <c r="X9" s="112"/>
       <c r="Y9" s="112"/>
     </row>
-    <row r="10" spans="1:25" ht="12.5">
+    <row r="10" spans="1:25" ht="12.75">
       <c r="A10" s="112"/>
       <c r="B10" s="164" t="s">
         <v>187</v>
@@ -9365,7 +9372,7 @@
       <c r="X11" s="112"/>
       <c r="Y11" s="118"/>
     </row>
-    <row r="12" spans="1:25" ht="12.5">
+    <row r="12" spans="1:25" ht="12.75">
       <c r="A12" s="112"/>
       <c r="B12" s="164" t="s">
         <v>255</v>
@@ -9432,7 +9439,7 @@
       <c r="X12" s="112"/>
       <c r="Y12" s="118"/>
     </row>
-    <row r="13" spans="1:25" ht="12.5">
+    <row r="13" spans="1:25" ht="12.75">
       <c r="A13" s="112"/>
       <c r="B13" s="164"/>
       <c r="C13" s="131"/>
@@ -9464,7 +9471,7 @@
       <c r="X13" s="112"/>
       <c r="Y13" s="118"/>
     </row>
-    <row r="14" spans="1:25" ht="12.5">
+    <row r="14" spans="1:25" ht="12.75">
       <c r="A14" s="112"/>
       <c r="B14" s="164"/>
       <c r="C14" s="131"/>
@@ -9513,7 +9520,7 @@
       <c r="X14" s="112"/>
       <c r="Y14" s="118"/>
     </row>
-    <row r="15" spans="1:25" ht="12.5">
+    <row r="15" spans="1:25" ht="12.75">
       <c r="A15" s="112"/>
       <c r="B15" s="164"/>
       <c r="C15" s="131"/>
@@ -9562,7 +9569,7 @@
       <c r="X15" s="112"/>
       <c r="Y15" s="118"/>
     </row>
-    <row r="16" spans="1:25" ht="12.5">
+    <row r="16" spans="1:25" ht="12.75">
       <c r="A16" s="112"/>
       <c r="B16" s="165"/>
       <c r="C16" s="112"/>
@@ -9612,7 +9619,7 @@
       <c r="X16" s="112"/>
       <c r="Y16" s="112"/>
     </row>
-    <row r="17" spans="1:25" ht="12.5">
+    <row r="17" spans="1:25" ht="12.75">
       <c r="A17" s="112"/>
       <c r="B17" s="165"/>
       <c r="C17" s="112"/>
@@ -9653,7 +9660,7 @@
       <c r="X17" s="112"/>
       <c r="Y17" s="112"/>
     </row>
-    <row r="18" spans="1:25" ht="12.5">
+    <row r="18" spans="1:25" ht="12.75">
       <c r="A18" s="112"/>
       <c r="B18" s="165"/>
       <c r="C18" s="112"/>
@@ -9680,7 +9687,7 @@
       <c r="X18" s="112"/>
       <c r="Y18" s="112"/>
     </row>
-    <row r="19" spans="1:25" ht="12.5">
+    <row r="19" spans="1:25" ht="12.75">
       <c r="A19" s="112"/>
       <c r="B19" s="165"/>
       <c r="C19" s="112"/>
@@ -9709,7 +9716,7 @@
       <c r="X19" s="112"/>
       <c r="Y19" s="112"/>
     </row>
-    <row r="20" spans="1:25" ht="37.5">
+    <row r="20" spans="1:25" ht="38.25">
       <c r="A20" s="115"/>
       <c r="B20" s="163" t="s">
         <v>189</v>
@@ -9748,7 +9755,7 @@
       <c r="X20" s="115"/>
       <c r="Y20" s="115"/>
     </row>
-    <row r="21" spans="1:25" ht="12.5">
+    <row r="21" spans="1:25" ht="12.75">
       <c r="A21" s="112"/>
       <c r="B21" s="164" t="s">
         <v>162</v>
@@ -9824,7 +9831,7 @@
       <c r="X21" s="112"/>
       <c r="Y21" s="112"/>
     </row>
-    <row r="22" spans="1:25" ht="12.5">
+    <row r="22" spans="1:25" ht="12.75">
       <c r="A22" s="112"/>
       <c r="B22" s="164" t="s">
         <v>194</v>
@@ -9884,7 +9891,7 @@
       <c r="X22" s="112"/>
       <c r="Y22" s="118"/>
     </row>
-    <row r="23" spans="1:25" ht="12.5">
+    <row r="23" spans="1:25" ht="12.75">
       <c r="A23" s="112"/>
       <c r="B23" s="164" t="s">
         <v>195</v>
@@ -9945,7 +9952,7 @@
       <c r="X23" s="112"/>
       <c r="Y23" s="112"/>
     </row>
-    <row r="24" spans="1:25" ht="12.5">
+    <row r="24" spans="1:25" ht="12.75">
       <c r="A24" s="112"/>
       <c r="B24" s="164" t="s">
         <v>196</v>
@@ -10013,7 +10020,7 @@
       <c r="X24" s="112"/>
       <c r="Y24" s="112"/>
     </row>
-    <row r="25" spans="1:25" ht="12.5">
+    <row r="25" spans="1:25" ht="12.75">
       <c r="A25" s="112"/>
       <c r="B25" s="164" t="s">
         <v>197</v>
@@ -10081,7 +10088,7 @@
       <c r="X25" s="112"/>
       <c r="Y25" s="112"/>
     </row>
-    <row r="26" spans="1:25" ht="12.5">
+    <row r="26" spans="1:25" ht="12.75">
       <c r="A26" s="112"/>
       <c r="B26" s="164" t="s">
         <v>198</v>
@@ -10147,7 +10154,7 @@
       <c r="X26" s="112"/>
       <c r="Y26" s="112"/>
     </row>
-    <row r="27" spans="1:25" ht="12.5">
+    <row r="27" spans="1:25" ht="12.75">
       <c r="A27" s="112"/>
       <c r="B27" s="164" t="s">
         <v>199</v>
@@ -10199,7 +10206,7 @@
       <c r="X27" s="112"/>
       <c r="Y27" s="112"/>
     </row>
-    <row r="28" spans="1:25" ht="12.5">
+    <row r="28" spans="1:25" ht="12.75">
       <c r="A28" s="112"/>
       <c r="B28" s="164" t="s">
         <v>200</v>
@@ -10251,7 +10258,7 @@
       <c r="X28" s="112"/>
       <c r="Y28" s="112"/>
     </row>
-    <row r="29" spans="1:25" ht="12.5">
+    <row r="29" spans="1:25" ht="12.75">
       <c r="A29" s="112"/>
       <c r="B29" s="165"/>
       <c r="C29" s="112"/>
@@ -10284,7 +10291,7 @@
       <c r="X29" s="112"/>
       <c r="Y29" s="112"/>
     </row>
-    <row r="30" spans="1:25" ht="12.5">
+    <row r="30" spans="1:25" ht="12.75">
       <c r="A30" s="112"/>
       <c r="B30" s="164"/>
       <c r="C30" s="112"/>
@@ -10334,7 +10341,7 @@
       <c r="X30" s="112"/>
       <c r="Y30" s="112"/>
     </row>
-    <row r="31" spans="1:25" ht="12.5">
+    <row r="31" spans="1:25" ht="12.75">
       <c r="A31" s="112"/>
       <c r="B31" s="164"/>
       <c r="C31" s="112"/>
@@ -10375,7 +10382,7 @@
       <c r="X31" s="112"/>
       <c r="Y31" s="112"/>
     </row>
-    <row r="32" spans="1:25" ht="12.5">
+    <row r="32" spans="1:25" ht="12.75">
       <c r="A32" s="112"/>
       <c r="B32" s="164"/>
       <c r="C32" s="112"/>
@@ -10402,7 +10409,7 @@
       <c r="X32" s="112"/>
       <c r="Y32" s="112"/>
     </row>
-    <row r="33" spans="1:25" ht="12.5">
+    <row r="33" spans="1:25" ht="12.75">
       <c r="A33" s="112"/>
       <c r="B33" s="164"/>
       <c r="C33" s="112"/>
@@ -10429,15 +10436,15 @@
       <c r="X33" s="112"/>
       <c r="Y33" s="112"/>
     </row>
-    <row r="34" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="34" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B34" s="165"/>
     </row>
-    <row r="35" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="35" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B35" s="164" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="36" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B36" s="164" t="s">
         <v>217</v>
       </c>
@@ -10445,7 +10452,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="37" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B37" s="164" t="s">
         <v>219</v>
       </c>
@@ -10453,10 +10460,10 @@
         <v>220</v>
       </c>
     </row>
-    <row r="38" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="38" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B38" s="165"/>
     </row>
-    <row r="39" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="39" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B39" s="164" t="s">
         <v>226</v>
       </c>
@@ -10464,7 +10471,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="40" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="40" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B40" s="164" t="s">
         <v>223</v>
       </c>
@@ -10472,7 +10479,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="41" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="41" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B41" s="164" t="s">
         <v>225</v>
       </c>
@@ -10480,10 +10487,10 @@
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="42" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B42" s="166"/>
     </row>
-    <row r="43" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="43" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B43" s="164" t="s">
         <v>229</v>
       </c>
@@ -10491,7 +10498,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="44" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="44" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B44" s="164" t="s">
         <v>231</v>
       </c>
@@ -10499,7 +10506,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="45" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B45" s="164" t="s">
         <v>275</v>
       </c>
@@ -10507,10 +10514,10 @@
         <v>276</v>
       </c>
     </row>
-    <row r="46" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="46" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B46" s="166"/>
     </row>
-    <row r="47" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="47" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B47" s="164" t="s">
         <v>234</v>
       </c>
@@ -10518,7 +10525,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="48" spans="1:25" s="112" customFormat="1" ht="12.5">
+    <row r="48" spans="1:25" s="112" customFormat="1" ht="12.75">
       <c r="B48" s="164" t="s">
         <v>233</v>
       </c>
@@ -10526,7 +10533,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="49" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="49" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B49" s="164" t="s">
         <v>277</v>
       </c>
@@ -10534,13 +10541,13 @@
         <v>278</v>
       </c>
     </row>
-    <row r="50" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="50" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B50" s="164"/>
     </row>
-    <row r="51" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="51" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B51" s="164"/>
     </row>
-    <row r="52" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="52" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B52" s="164" t="s">
         <v>237</v>
       </c>
@@ -10548,7 +10555,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="53" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B53" s="164" t="s">
         <v>238</v>
       </c>
@@ -10556,7 +10563,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="54" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="54" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B54" s="164" t="s">
         <v>243</v>
       </c>
@@ -10564,7 +10571,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="55" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="55" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B55" s="164" t="s">
         <v>245</v>
       </c>
@@ -10572,10 +10579,10 @@
         <v>246</v>
       </c>
     </row>
-    <row r="56" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="56" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B56" s="164"/>
     </row>
-    <row r="57" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="57" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B57" s="164" t="s">
         <v>252</v>
       </c>
@@ -10583,7 +10590,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="58" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="58" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B58" s="164" t="s">
         <v>247</v>
       </c>
@@ -10591,7 +10598,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="59" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="59" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B59" s="164" t="s">
         <v>249</v>
       </c>
@@ -10599,7 +10606,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="60" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="60" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B60" s="164" t="s">
         <v>250</v>
       </c>
@@ -10607,10 +10614,10 @@
         <v>254</v>
       </c>
     </row>
-    <row r="61" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="61" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B61" s="164"/>
     </row>
-    <row r="62" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="62" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B62" s="164" t="s">
         <v>256</v>
       </c>
@@ -10618,7 +10625,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="63" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="63" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B63" s="164" t="s">
         <v>257</v>
       </c>
@@ -10626,7 +10633,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="64" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="64" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B64" s="164" t="s">
         <v>258</v>
       </c>
@@ -10634,7 +10641,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="65" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="65" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B65" s="164" t="s">
         <v>259</v>
       </c>
@@ -10642,7 +10649,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="66" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="66" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B66" s="164" t="s">
         <v>260</v>
       </c>
@@ -10650,10 +10657,10 @@
         <v>265</v>
       </c>
     </row>
-    <row r="67" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="67" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B67" s="164"/>
     </row>
-    <row r="68" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="68" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B68" s="164" t="s">
         <v>266</v>
       </c>
@@ -10661,7 +10668,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="69" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="69" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B69" s="164" t="s">
         <v>268</v>
       </c>
@@ -10669,10 +10676,10 @@
         <v>269</v>
       </c>
     </row>
-    <row r="70" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="70" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B70" s="164"/>
     </row>
-    <row r="71" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="71" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B71" s="164" t="s">
         <v>272</v>
       </c>
@@ -10680,7 +10687,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="72" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="72" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B72" s="164" t="s">
         <v>270</v>
       </c>
@@ -10688,7 +10695,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="73" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="73" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B73" s="164" t="s">
         <v>274</v>
       </c>
@@ -10696,10 +10703,10 @@
         <v>279</v>
       </c>
     </row>
-    <row r="74" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="74" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B74" s="164"/>
     </row>
-    <row r="75" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="75" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B75" s="164" t="s">
         <v>281</v>
       </c>
@@ -10707,7 +10714,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="76" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="76" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B76" s="164" t="s">
         <v>280</v>
       </c>
@@ -10715,7 +10722,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="77" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="77" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B77" s="164" t="s">
         <v>282</v>
       </c>
@@ -10723,7 +10730,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="78" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="78" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B78" s="164" t="s">
         <v>284</v>
       </c>
@@ -10731,7 +10738,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="79" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="79" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B79" s="164" t="s">
         <v>285</v>
       </c>
@@ -10739,10 +10746,10 @@
         <v>286</v>
       </c>
     </row>
-    <row r="80" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="80" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B80" s="164"/>
     </row>
-    <row r="81" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="81" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B81" s="164" t="s">
         <v>287</v>
       </c>
@@ -10750,7 +10757,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="82" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="82" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B82" s="164" t="s">
         <v>288</v>
       </c>
@@ -10758,7 +10765,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="83" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="83" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B83" s="164" t="s">
         <v>289</v>
       </c>
@@ -10766,7 +10773,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="84" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="84" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B84" s="164" t="s">
         <v>290</v>
       </c>
@@ -10774,7 +10781,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="85" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="85" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B85" s="164" t="s">
         <v>291</v>
       </c>
@@ -10782,10 +10789,10 @@
         <v>286</v>
       </c>
     </row>
-    <row r="86" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="86" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B86" s="164"/>
     </row>
-    <row r="87" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="87" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B87" s="164" t="s">
         <v>294</v>
       </c>
@@ -10793,7 +10800,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="88" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="88" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B88" s="164" t="s">
         <v>296</v>
       </c>
@@ -10801,7 +10808,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="89" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="89" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B89" s="164" t="s">
         <v>297</v>
       </c>
@@ -10809,7 +10816,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="90" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="90" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B90" s="164" t="s">
         <v>300</v>
       </c>
@@ -10817,7 +10824,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="91" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="91" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B91" s="164" t="s">
         <v>302</v>
       </c>
@@ -10825,8 +10832,8 @@
         <v>286</v>
       </c>
     </row>
-    <row r="92" spans="2:3" s="112" customFormat="1" ht="12.5"/>
-    <row r="93" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="92" spans="2:3" s="112" customFormat="1" ht="12.75"/>
+    <row r="93" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B93" s="164" t="s">
         <v>199</v>
       </c>
@@ -10834,7 +10841,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="94" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="94" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B94" s="164" t="s">
         <v>200</v>
       </c>
@@ -10842,10 +10849,10 @@
         <v>303</v>
       </c>
     </row>
-    <row r="95" spans="2:3" s="112" customFormat="1" ht="12.5">
+    <row r="95" spans="2:3" s="112" customFormat="1" ht="12.75">
       <c r="B95" s="165"/>
     </row>
-    <row r="96" spans="2:3" ht="12.5">
+    <row r="96" spans="2:3" ht="12.75">
       <c r="B96" s="164" t="s">
         <v>221</v>
       </c>
@@ -10977,9 +10984,9 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col min="2" max="7" width="15.77734375" customWidth="1"/>
+    <col min="2" max="7" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -11662,18 +11669,18 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="18" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="23" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12663,13 +12670,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -12756,7 +12763,7 @@
         <f>'Main Page'!$B$29</f>
         <v>28.647889756541161</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>464</v>
       </c>
       <c r="K8" s="380"/>
@@ -12772,7 +12779,7 @@
         <f>'Main Page'!$B$34</f>
         <v>2.6</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>465</v>
       </c>
       <c r="K9" s="380"/>
@@ -12788,7 +12795,7 @@
         <f>'Main Page'!$B$35</f>
         <v>90</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>466</v>
       </c>
       <c r="K10" s="380"/>
@@ -12804,7 +12811,7 @@
         <f>'Main Page'!$B$40</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>467</v>
       </c>
       <c r="K11" s="380"/>
@@ -12820,7 +12827,7 @@
         <f>'Main Page'!$B$37*PI()/180</f>
         <v>4.5378560551852569E-2</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>468</v>
       </c>
       <c r="K12" s="380"/>
@@ -12836,7 +12843,7 @@
         <f>'Main Page'!$B$38*PI()/180</f>
         <v>0.52359877559829882</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>469</v>
       </c>
       <c r="K13" s="380"/>
@@ -12852,7 +12859,7 @@
         <f>1/C12^C15</f>
         <v>0.21302244142778143</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>470</v>
       </c>
       <c r="K14" s="380"/>
@@ -12868,27 +12875,60 @@
         <f>'Main Page'!$B$39</f>
         <v>-0.5</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>471</v>
       </c>
       <c r="K15" s="380"/>
     </row>
     <row r="16" spans="1:14">
+      <c r="B16" t="s">
+        <v>511</v>
+      </c>
+      <c r="C16" s="101">
+        <f>(4*'Main Page'!$B$29/30*PI())^2</f>
+        <v>144</v>
+      </c>
+      <c r="D16" s="101">
+        <v>0</v>
+      </c>
+      <c r="E16" s="101">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>513</v>
+      </c>
       <c r="K16" s="380"/>
     </row>
-    <row r="17" spans="11:11">
+    <row r="17" spans="2:11">
+      <c r="B17" t="s">
+        <v>512</v>
+      </c>
+      <c r="C17" s="101">
+        <f>(4*'Main Page'!$B$29/30*PI())^2</f>
+        <v>144</v>
+      </c>
+      <c r="D17" s="101">
+        <f>2*0.8*(4*'Main Page'!$B$29/30*PI())</f>
+        <v>19.200000000000003</v>
+      </c>
+      <c r="E17" s="101">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>514</v>
+      </c>
       <c r="K17" s="102"/>
     </row>
-    <row r="19" spans="11:11">
+    <row r="19" spans="2:11">
       <c r="K19" s="381"/>
     </row>
-    <row r="20" spans="11:11">
+    <row r="20" spans="2:11">
       <c r="K20" s="102"/>
     </row>
-    <row r="21" spans="11:11">
+    <row r="21" spans="2:11">
       <c r="K21" s="102"/>
     </row>
-    <row r="22" spans="11:11">
+    <row r="22" spans="2:11">
       <c r="K22" s="102"/>
     </row>
   </sheetData>
@@ -12904,12 +12944,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -13178,14 +13218,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="15.77734375" customWidth="1"/>
+    <col min="3" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -13539,18 +13579,18 @@
       <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="17" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="16" style="18" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="11" width="12.44140625" customWidth="1"/>
+    <col min="10" max="11" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="13.5" thickBot="1">
@@ -13558,7 +13598,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="11" thickBot="1">
+    <row r="2" spans="1:11" ht="12" thickBot="1">
       <c r="A2" s="409" t="s">
         <v>84</v>
       </c>
@@ -13590,7 +13630,7 @@
       <c r="G3" s="77"/>
       <c r="H3" s="78"/>
     </row>
-    <row r="4" spans="1:11" ht="11" thickBot="1">
+    <row r="4" spans="1:11" ht="12" thickBot="1">
       <c r="A4" s="263">
         <v>0.01</v>
       </c>
@@ -13618,7 +13658,7 @@
       <c r="D6" s="59"/>
       <c r="E6" s="57"/>
     </row>
-    <row r="7" spans="1:11" s="19" customFormat="1" ht="32.5" customHeight="1" thickBot="1">
+    <row r="7" spans="1:11" s="19" customFormat="1" ht="32.450000000000003" customHeight="1" thickBot="1">
       <c r="A7" s="45" t="s">
         <v>1</v>
       </c>
@@ -13653,7 +13693,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="10.5" thickBot="1">
+    <row r="8" spans="1:11" ht="12" thickBot="1">
       <c r="A8" s="47">
         <v>1</v>
       </c>
@@ -13696,7 +13736,7 @@
         <v>62126221909.368462</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="10.5" thickBot="1">
+    <row r="9" spans="1:11" ht="12" thickBot="1">
       <c r="A9" s="48">
         <v>2</v>
       </c>
@@ -13739,7 +13779,7 @@
         <v>50601045349.013542</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="10.5" thickBot="1">
+    <row r="10" spans="1:11" ht="12" thickBot="1">
       <c r="A10" s="48">
         <v>3</v>
       </c>
@@ -13782,7 +13822,7 @@
         <v>40756895137.180222</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="10.5" thickBot="1">
+    <row r="11" spans="1:11" ht="12" thickBot="1">
       <c r="A11" s="48">
         <v>4</v>
       </c>
@@ -13825,7 +13865,7 @@
         <v>32422036127.620483</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="10.5" thickBot="1">
+    <row r="12" spans="1:11" ht="12" thickBot="1">
       <c r="A12" s="48">
         <v>5</v>
       </c>
@@ -13868,7 +13908,7 @@
         <v>25433971568.120796</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="10.5" thickBot="1">
+    <row r="13" spans="1:11" ht="12" thickBot="1">
       <c r="A13" s="48">
         <v>6</v>
       </c>
@@ -13911,7 +13951,7 @@
         <v>19639443100.502033</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="10.5" thickBot="1">
+    <row r="14" spans="1:11" ht="12" thickBot="1">
       <c r="A14" s="48">
         <v>7</v>
       </c>
@@ -13954,7 +13994,7 @@
         <v>14894430760.619625</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="10.5" thickBot="1">
+    <row r="15" spans="1:11" ht="12" thickBot="1">
       <c r="A15" s="48">
         <v>8</v>
       </c>
@@ -13997,7 +14037,7 @@
         <v>11064152978.363453</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="10.5" thickBot="1">
+    <row r="16" spans="1:11" ht="12" thickBot="1">
       <c r="A16" s="48">
         <v>9</v>
       </c>
@@ -14293,7 +14333,7 @@
       <c r="J31" s="29"/>
       <c r="K31" s="30"/>
     </row>
-    <row r="32" spans="1:11" ht="10.5" thickBot="1">
+    <row r="32" spans="1:11" ht="12" thickBot="1">
       <c r="A32" s="49">
         <v>25</v>
       </c>
@@ -14330,33 +14370,33 @@
       <selection activeCell="D2" sqref="D2:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="7.5" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="11.5" customWidth="1"/>
     <col min="13" max="13" width="12.33203125" customWidth="1"/>
     <col min="14" max="14" width="11.6640625" customWidth="1"/>
     <col min="15" max="15" width="7.33203125" customWidth="1"/>
-    <col min="16" max="16" width="10.44140625" customWidth="1"/>
-    <col min="17" max="17" width="15.44140625" customWidth="1"/>
+    <col min="16" max="16" width="10.5" customWidth="1"/>
+    <col min="17" max="17" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.65" customHeight="1" thickBot="1">
+    <row r="1" spans="1:20" ht="15.6" customHeight="1" thickBot="1">
       <c r="A1" s="55" t="s">
         <v>64</v>
       </c>
       <c r="B1" s="57"/>
     </row>
-    <row r="2" spans="1:20" ht="20.5" thickBot="1">
+    <row r="2" spans="1:20" ht="23.25" thickBot="1">
       <c r="A2" s="96" t="s">
         <v>56</v>
       </c>
@@ -14370,7 +14410,7 @@
       <c r="E2" s="397"/>
       <c r="F2" s="398"/>
     </row>
-    <row r="3" spans="1:20" ht="20.5" thickBot="1">
+    <row r="3" spans="1:20" ht="23.25" thickBot="1">
       <c r="A3" s="98" t="s">
         <v>57</v>
       </c>
@@ -14393,7 +14433,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:20" ht="11" thickBot="1">
+    <row r="4" spans="1:20" ht="12" thickBot="1">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="D4" s="263">
@@ -14411,7 +14451,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:20" ht="10.5">
+    <row r="5" spans="1:20">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="F5" s="4"/>
@@ -14421,7 +14461,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:20" ht="13">
+    <row r="6" spans="1:20" ht="12.75">
       <c r="A6" s="55" t="s">
         <v>32</v>
       </c>
@@ -14435,7 +14475,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:20" ht="10.5">
+    <row r="7" spans="1:20">
       <c r="A7" s="52" t="s">
         <v>34</v>
       </c>
@@ -14447,7 +14487,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:20" s="5" customFormat="1" ht="10.5">
+    <row r="8" spans="1:20" s="5" customFormat="1">
       <c r="A8" s="13" t="s">
         <v>27</v>
       </c>
@@ -14468,7 +14508,7 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" spans="1:20" s="19" customFormat="1" ht="30">
+    <row r="9" spans="1:20" s="19" customFormat="1" ht="33.75">
       <c r="A9" s="87" t="s">
         <v>0</v>
       </c>
@@ -16125,7 +16165,7 @@
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
     </row>
-    <row r="32" spans="1:20" ht="10.5">
+    <row r="32" spans="1:20">
       <c r="A32" s="7">
         <v>23</v>
       </c>
@@ -16544,27 +16584,27 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" customWidth="1"/>
     <col min="13" max="13" width="10.33203125" customWidth="1"/>
     <col min="14" max="14" width="12.33203125" customWidth="1"/>
-    <col min="15" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.44140625" customWidth="1"/>
+    <col min="15" max="16" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5" customWidth="1"/>
     <col min="19" max="19" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="27" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:21">

</xml_diff>

<commit_message>
Updating method for loading/creating turbines
Trying to use more of jr_fast functions
</commit_message>
<xml_diff>
--- a/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
+++ b/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="705" windowWidth="17565" windowHeight="12990" activeTab="3"/>
+    <workbookView xWindow="1560" yWindow="705" windowWidth="17565" windowHeight="12990"/>
   </bookViews>
   <sheets>
     <sheet name="Main Page" sheetId="5" r:id="rId1"/>
@@ -4479,11 +4479,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95175808"/>
-        <c:axId val="95177728"/>
+        <c:axId val="96953472"/>
+        <c:axId val="96955392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95175808"/>
+        <c:axId val="96953472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4568,12 +4568,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95177728"/>
+        <c:crossAx val="96955392"/>
         <c:crossesAt val="-10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95177728"/>
+        <c:axId val="96955392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4657,7 +4657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95175808"/>
+        <c:crossAx val="96953472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5733,8 +5733,8 @@
   </sheetPr>
   <dimension ref="A1:U158"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -10980,7 +10980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -11665,8 +11665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -12670,7 +12670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -12941,7 +12941,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -13219,7 +13219,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>

</xml_diff>

<commit_message>
Updating turbine dictionary/writing technique, regen'd turb files
</commit_message>
<xml_diff>
--- a/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
+++ b/FAST_models/WindPACT/excel_proc/turbines/0.75A08V00_proc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="705" windowWidth="17565" windowHeight="12990"/>
+    <workbookView xWindow="1560" yWindow="705" windowWidth="17565" windowHeight="12990" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Main Page" sheetId="5" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="525">
   <si>
     <t>number</t>
   </si>
@@ -1732,12 +1732,6 @@
     <t>Cylinder changed to produce correct AeroCent (JR)</t>
   </si>
   <si>
-    <t>RotorDiameter</t>
-  </si>
-  <si>
-    <t>HubDiameter</t>
-  </si>
-  <si>
     <t>BladeDamping (%)</t>
   </si>
   <si>
@@ -1804,9 +1798,6 @@
     <t>FoilNm</t>
   </si>
   <si>
-    <t>BldDmp</t>
-  </si>
-  <si>
     <t>BlFract</t>
   </si>
   <si>
@@ -1831,9 +1822,6 @@
     <t>deg</t>
   </si>
   <si>
-    <t>PreCone</t>
-  </si>
-  <si>
     <t>ShftTilt</t>
   </si>
   <si>
@@ -1951,9 +1939,6 @@
     <t>RatedPwr</t>
   </si>
   <si>
-    <t>TwrDmp</t>
-  </si>
-  <si>
     <t>TwrSchedFields</t>
   </si>
   <si>
@@ -2023,9 +2008,6 @@
     <t>ADSched Calculations</t>
   </si>
   <si>
-    <t>BlPitchF</t>
-  </si>
-  <si>
     <t>N-m</t>
   </si>
   <si>
@@ -2051,6 +2033,45 @@
   </si>
   <si>
     <t>&lt;-- added ".dat" (JR)</t>
+  </si>
+  <si>
+    <t>BldFlDmp(1)</t>
+  </si>
+  <si>
+    <t>BldFlDmp(2)</t>
+  </si>
+  <si>
+    <t>BldEdDmp(1)</t>
+  </si>
+  <si>
+    <t>BlPitchF(1)</t>
+  </si>
+  <si>
+    <t>BlPitchF(2)</t>
+  </si>
+  <si>
+    <t>BlPitchF(3)</t>
+  </si>
+  <si>
+    <t>TwrFADmp(1)</t>
+  </si>
+  <si>
+    <t>TwrFADmp(2)</t>
+  </si>
+  <si>
+    <t>TwrSSDmp(1)</t>
+  </si>
+  <si>
+    <t>TwrSSDmp(2)</t>
+  </si>
+  <si>
+    <t>PreCone(1)</t>
+  </si>
+  <si>
+    <t>PreCone(2)</t>
+  </si>
+  <si>
+    <t>PreCone(3)</t>
   </si>
 </sst>
 </file>
@@ -4488,11 +4509,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="104359040"/>
-        <c:axId val="104360960"/>
+        <c:axId val="112813184"/>
+        <c:axId val="112815104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104359040"/>
+        <c:axId val="112813184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4577,12 +4598,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104360960"/>
+        <c:crossAx val="112815104"/>
         <c:crossesAt val="-10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104360960"/>
+        <c:axId val="112815104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4666,7 +4687,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104359040"/>
+        <c:crossAx val="112813184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5742,8 +5763,8 @@
   </sheetPr>
   <dimension ref="A1:U158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I141" sqref="I141"/>
+    <sheetView topLeftCell="A115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H139" sqref="H139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -6013,13 +6034,13 @@
         <v>129646444.93189973</v>
       </c>
       <c r="D14" s="352" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E14" s="353"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="61" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B15" s="378">
         <v>5</v>
@@ -6031,7 +6052,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="61" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B16" s="378">
         <v>665139</v>
@@ -6249,7 +6270,7 @@
         <v>4188.2879761025097</v>
       </c>
       <c r="D31" s="352" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E31" s="353"/>
     </row>
@@ -6288,49 +6309,49 @@
     </row>
     <row r="37" spans="1:5" ht="12" customHeight="1">
       <c r="A37" s="379" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B37" s="273">
         <v>2.6</v>
       </c>
       <c r="D37" s="352" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E37" s="353"/>
     </row>
     <row r="38" spans="1:5" ht="12" customHeight="1">
       <c r="A38" s="379" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B38" s="273">
         <v>30</v>
       </c>
       <c r="D38" s="352" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E38" s="353"/>
     </row>
     <row r="39" spans="1:5" ht="12" customHeight="1">
       <c r="A39" s="379" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B39" s="273">
         <v>-0.5</v>
       </c>
       <c r="D39" s="352" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E39" s="353"/>
     </row>
     <row r="40" spans="1:5" ht="12" customHeight="1">
       <c r="A40" s="379" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B40" s="273">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D40" s="352" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E40" s="353"/>
     </row>
@@ -6348,14 +6369,14 @@
     </row>
     <row r="43" spans="1:5" ht="12" customHeight="1">
       <c r="A43" s="379" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B43" s="273">
         <f>B31/B87^2</f>
         <v>1.2926814741057128E-3</v>
       </c>
       <c r="D43" s="352" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E43" s="353"/>
     </row>
@@ -7258,7 +7279,7 @@
         <v>89</v>
       </c>
       <c r="E122" s="384" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="F122" s="188" t="s">
         <v>324</v>
@@ -7267,7 +7288,7 @@
         <v>325</v>
       </c>
       <c r="H122" s="384" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I122" s="188" t="s">
         <v>342</v>
@@ -7595,7 +7616,7 @@
         <v>363</v>
       </c>
       <c r="C134" s="385" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D134" s="392"/>
     </row>
@@ -7702,10 +7723,10 @@
       </c>
       <c r="B144" s="342"/>
       <c r="C144" s="343" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="E144" s="352" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="F144" s="353"/>
     </row>
@@ -11003,13 +11024,13 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" t="s">
         <v>427</v>
-      </c>
-      <c r="B1" t="s">
-        <v>428</v>
-      </c>
-      <c r="C1" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -11017,7 +11038,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C3" s="18">
         <f>'Main Page'!B17</f>
@@ -11026,10 +11047,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B4" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="C4">
         <v>5.0000000000000001E-3</v>
@@ -11037,10 +11058,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C5" s="18" t="str">
         <f>'Main Page'!C144</f>
@@ -11061,10 +11082,10 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B6" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C6" s="18">
         <v>15</v>
@@ -11075,25 +11096,25 @@
     </row>
     <row r="7" spans="1:8">
       <c r="B7" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="C7" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="D7" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="E7" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="F7" t="s">
         <v>88</v>
       </c>
       <c r="G7" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="H7" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -11118,7 +11139,7 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -11143,7 +11164,7 @@
         <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -11168,7 +11189,7 @@
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -11193,7 +11214,7 @@
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -11218,7 +11239,7 @@
         <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -11243,7 +11264,7 @@
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -11268,7 +11289,7 @@
         <v>2</v>
       </c>
       <c r="H14" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -11293,7 +11314,7 @@
         <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -11318,7 +11339,7 @@
         <v>3</v>
       </c>
       <c r="H16" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="17" spans="3:8">
@@ -11343,7 +11364,7 @@
         <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="18" spans="3:8">
@@ -11368,7 +11389,7 @@
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="19" spans="3:8">
@@ -11393,7 +11414,7 @@
         <v>3</v>
       </c>
       <c r="H19" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="20" spans="3:8">
@@ -11418,7 +11439,7 @@
         <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="21" spans="3:8">
@@ -11443,7 +11464,7 @@
         <v>4</v>
       </c>
       <c r="H21" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="22" spans="3:8">
@@ -11468,12 +11489,12 @@
         <v>4</v>
       </c>
       <c r="H22" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="36" spans="2:7">
       <c r="B36" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="E36" t="s">
         <v>88</v>
@@ -11726,7 +11747,7 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="B3" sqref="B3:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -11746,28 +11767,26 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" t="s">
         <v>427</v>
-      </c>
-      <c r="B1" t="s">
-        <v>428</v>
-      </c>
-      <c r="C1" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>385</v>
       </c>
       <c r="B3" t="s">
-        <v>432</v>
+        <v>512</v>
       </c>
       <c r="C3" s="18">
-        <f>'Main Page'!B13/2</f>
-        <v>25</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+        <f>'Main Page'!A151*100</f>
+        <v>3.8820000000000001</v>
+      </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
@@ -11786,23 +11805,20 @@
       <c r="U3" s="18"/>
       <c r="V3" s="18"/>
       <c r="W3" s="18"/>
-      <c r="Y3" t="s">
+      <c r="Y3" s="358" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="4" spans="1:25">
-      <c r="A4" t="s">
-        <v>85</v>
-      </c>
       <c r="B4" t="s">
-        <v>433</v>
+        <v>513</v>
       </c>
       <c r="C4" s="18">
-        <f>'Main Page'!B56/2</f>
-        <v>1.25</v>
+        <f>'Main Page'!B151*100</f>
+        <v>3.8820000000000001</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="E4" s="386"/>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
@@ -11821,29 +11837,18 @@
       <c r="U4" s="18"/>
       <c r="V4" s="18"/>
       <c r="W4" s="18"/>
-      <c r="Y4" t="s">
-        <v>412</v>
-      </c>
+      <c r="Y4" s="358"/>
     </row>
     <row r="5" spans="1:25">
-      <c r="A5" t="s">
-        <v>385</v>
-      </c>
       <c r="B5" t="s">
-        <v>435</v>
-      </c>
-      <c r="C5" s="18">
-        <f>'Main Page'!A151*100</f>
-        <v>3.8820000000000001</v>
-      </c>
-      <c r="D5" s="18">
-        <f>'Main Page'!B151*100</f>
-        <v>3.8820000000000001</v>
-      </c>
-      <c r="E5" s="386">
+        <v>514</v>
+      </c>
+      <c r="C5" s="386">
         <f>'Main Page'!C151*100</f>
         <v>5.8999999999999995</v>
       </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="386"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
@@ -11862,37 +11867,35 @@
       <c r="U5" s="18"/>
       <c r="V5" s="18"/>
       <c r="W5" s="18"/>
-      <c r="Y5" s="358" t="s">
-        <v>413</v>
-      </c>
+      <c r="Y5" s="358"/>
     </row>
     <row r="6" spans="1:25">
       <c r="B6" t="s">
+        <v>487</v>
+      </c>
+      <c r="C6" s="387" t="s">
+        <v>433</v>
+      </c>
+      <c r="D6" s="387" t="s">
+        <v>488</v>
+      </c>
+      <c r="E6" s="387" t="s">
+        <v>489</v>
+      </c>
+      <c r="F6" s="387" t="s">
+        <v>490</v>
+      </c>
+      <c r="G6" s="387" t="s">
+        <v>491</v>
+      </c>
+      <c r="H6" s="387" t="s">
         <v>492</v>
       </c>
-      <c r="C6" s="387" t="s">
-        <v>436</v>
-      </c>
-      <c r="D6" s="387" t="s">
+      <c r="I6" s="387" t="s">
         <v>493</v>
       </c>
-      <c r="E6" s="387" t="s">
+      <c r="J6" s="387" t="s">
         <v>494</v>
-      </c>
-      <c r="F6" s="387" t="s">
-        <v>495</v>
-      </c>
-      <c r="G6" s="387" t="s">
-        <v>496</v>
-      </c>
-      <c r="H6" s="387" t="s">
-        <v>497</v>
-      </c>
-      <c r="I6" s="387" t="s">
-        <v>498</v>
-      </c>
-      <c r="J6" s="387" t="s">
-        <v>499</v>
       </c>
       <c r="K6" s="387"/>
       <c r="L6" s="387"/>
@@ -11908,7 +11911,7 @@
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
       <c r="Y6" s="358" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -12728,10 +12731,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N22"/>
+  <dimension ref="A2:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -12743,13 +12746,13 @@
   <sheetData>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B2" t="s">
+        <v>426</v>
+      </c>
+      <c r="C2" t="s">
         <v>427</v>
-      </c>
-      <c r="B2" t="s">
-        <v>428</v>
-      </c>
-      <c r="C2" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -12763,7 +12766,7 @@
         <v>394</v>
       </c>
       <c r="B4" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C4" s="101">
         <f>'Main Page'!B87</f>
@@ -12776,10 +12779,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="B5" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C5" s="381">
         <f>'Main Page'!$B$31</f>
@@ -12789,10 +12792,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B6" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C6" s="382">
         <f>'Main Page'!B43</f>
@@ -12802,10 +12805,10 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B7" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="C7" s="382">
         <v>2.6</v>
@@ -12814,182 +12817,206 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
+        <v>440</v>
+      </c>
+      <c r="B8" t="s">
+        <v>516</v>
+      </c>
+      <c r="C8" s="382">
+        <v>2.6</v>
+      </c>
+      <c r="K8" s="380"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>440</v>
+      </c>
+      <c r="B9" t="s">
+        <v>517</v>
+      </c>
+      <c r="C9" s="382">
+        <v>2.6</v>
+      </c>
+      <c r="K9" s="380"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
         <v>394</v>
       </c>
-      <c r="B8" t="s">
-        <v>453</v>
-      </c>
-      <c r="C8">
+      <c r="B10" t="s">
+        <v>449</v>
+      </c>
+      <c r="C10">
         <f>'Main Page'!$B$29</f>
         <v>28.647889756541161</v>
       </c>
-      <c r="G8" t="s">
-        <v>463</v>
-      </c>
-      <c r="K8" s="380"/>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" t="s">
-        <v>443</v>
-      </c>
-      <c r="B9" t="s">
-        <v>454</v>
-      </c>
-      <c r="C9" s="102">
+      <c r="G10" t="s">
+        <v>459</v>
+      </c>
+      <c r="K10" s="380"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>440</v>
+      </c>
+      <c r="B11" t="s">
+        <v>450</v>
+      </c>
+      <c r="C11" s="102">
         <f>'Main Page'!$B$34</f>
         <v>2.6</v>
       </c>
-      <c r="G9" t="s">
-        <v>464</v>
-      </c>
-      <c r="K9" s="380"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" t="s">
-        <v>443</v>
-      </c>
-      <c r="B10" t="s">
-        <v>455</v>
-      </c>
-      <c r="C10" s="102">
+      <c r="G11" t="s">
+        <v>460</v>
+      </c>
+      <c r="K11" s="380"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>440</v>
+      </c>
+      <c r="B12" t="s">
+        <v>451</v>
+      </c>
+      <c r="C12" s="102">
         <f>'Main Page'!$B$35</f>
         <v>90</v>
       </c>
-      <c r="G10" t="s">
-        <v>465</v>
-      </c>
-      <c r="K10" s="380"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" t="s">
+      <c r="G12" t="s">
         <v>461</v>
       </c>
-      <c r="B11" t="s">
-        <v>456</v>
-      </c>
-      <c r="C11">
+      <c r="K12" s="380"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>457</v>
+      </c>
+      <c r="B13" t="s">
+        <v>452</v>
+      </c>
+      <c r="C13">
         <f>'Main Page'!$B$40</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G11" t="s">
-        <v>466</v>
-      </c>
-      <c r="K11" s="380"/>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" t="s">
+      <c r="G13" t="s">
         <v>462</v>
       </c>
-      <c r="B12" t="s">
-        <v>457</v>
-      </c>
-      <c r="C12">
+      <c r="K13" s="380"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>458</v>
+      </c>
+      <c r="B14" t="s">
+        <v>453</v>
+      </c>
+      <c r="C14">
         <f>'Main Page'!$B$37*PI()/180</f>
         <v>4.5378560551852569E-2</v>
       </c>
-      <c r="G12" t="s">
-        <v>467</v>
-      </c>
-      <c r="K12" s="380"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" t="s">
-        <v>462</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="G14" t="s">
+        <v>463</v>
+      </c>
+      <c r="K14" s="380"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
         <v>458</v>
       </c>
-      <c r="C13">
+      <c r="B15" t="s">
+        <v>454</v>
+      </c>
+      <c r="C15">
         <f>'Main Page'!$B$38*PI()/180</f>
         <v>0.52359877559829882</v>
       </c>
-      <c r="G13" t="s">
-        <v>468</v>
-      </c>
-      <c r="K13" s="380"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" t="s">
-        <v>430</v>
-      </c>
-      <c r="B14" t="s">
-        <v>459</v>
-      </c>
-      <c r="C14">
-        <f>1/C12^C15</f>
+      <c r="G15" t="s">
+        <v>464</v>
+      </c>
+      <c r="K15" s="380"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>428</v>
+      </c>
+      <c r="B16" t="s">
+        <v>455</v>
+      </c>
+      <c r="C16">
+        <f>1/C14^C17</f>
         <v>0.21302244142778143</v>
       </c>
-      <c r="G14" t="s">
-        <v>469</v>
-      </c>
-      <c r="K14" s="380"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" t="s">
-        <v>430</v>
-      </c>
-      <c r="B15" t="s">
-        <v>460</v>
-      </c>
-      <c r="C15">
+      <c r="G16" t="s">
+        <v>465</v>
+      </c>
+      <c r="K16" s="380"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>428</v>
+      </c>
+      <c r="B17" t="s">
+        <v>456</v>
+      </c>
+      <c r="C17">
         <f>'Main Page'!$B$39</f>
         <v>-0.5</v>
       </c>
-      <c r="G15" t="s">
-        <v>470</v>
-      </c>
-      <c r="K15" s="380"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="B16" t="s">
-        <v>510</v>
-      </c>
-      <c r="C16" s="101">
+      <c r="G17" t="s">
+        <v>466</v>
+      </c>
+      <c r="K17" s="380"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="B18" t="s">
+        <v>504</v>
+      </c>
+      <c r="C18" s="101">
         <f>(4*'Main Page'!$B$29/30*PI())^2</f>
         <v>144</v>
       </c>
-      <c r="D16" s="101">
-        <v>0</v>
-      </c>
-      <c r="E16" s="101">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>512</v>
-      </c>
-      <c r="K16" s="380"/>
-    </row>
-    <row r="17" spans="2:11">
-      <c r="B17" t="s">
-        <v>511</v>
-      </c>
-      <c r="C17" s="101">
+      <c r="D18" s="101">
+        <v>0</v>
+      </c>
+      <c r="E18" s="101">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>506</v>
+      </c>
+      <c r="K18" s="380"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="B19" t="s">
+        <v>505</v>
+      </c>
+      <c r="C19" s="101">
         <f>(4*'Main Page'!$B$29/30*PI())^2</f>
         <v>144</v>
       </c>
-      <c r="D17" s="101">
+      <c r="D19" s="101">
         <f>2*0.8*(4*'Main Page'!$B$29/30*PI())</f>
         <v>19.200000000000003</v>
       </c>
-      <c r="E17" s="101">
+      <c r="E19" s="101">
         <v>1</v>
       </c>
-      <c r="G17" t="s">
-        <v>513</v>
-      </c>
-      <c r="K17" s="102"/>
-    </row>
-    <row r="19" spans="2:11">
-      <c r="K19" s="381"/>
-    </row>
-    <row r="20" spans="2:11">
-      <c r="K20" s="102"/>
-    </row>
-    <row r="21" spans="2:11">
-      <c r="K21" s="102"/>
-    </row>
-    <row r="22" spans="2:11">
+      <c r="G19" t="s">
+        <v>507</v>
+      </c>
+      <c r="K19" s="102"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="K21" s="381"/>
+    </row>
+    <row r="22" spans="1:11">
       <c r="K22" s="102"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="K23" s="102"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="K24" s="102"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12998,10 +13025,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -13014,13 +13041,13 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" t="s">
         <v>427</v>
-      </c>
-      <c r="B1" t="s">
-        <v>428</v>
-      </c>
-      <c r="C1" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -13028,7 +13055,7 @@
         <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C3" s="381">
         <f>'Main Page'!B61</f>
@@ -13040,10 +13067,10 @@
         <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C4" s="381">
-        <f>('Main Page'!B5*'Main Page'!E5+'Main Page'!B6*'Main Page'!E6+'Main Page'!B7*'Main Page'!E7)/C11</f>
+        <f>('Main Page'!B5*'Main Page'!E5+'Main Page'!B6*'Main Page'!E6+'Main Page'!B7*'Main Page'!E7)/C13</f>
         <v>-5.9950003076370724E-2</v>
       </c>
       <c r="I4" s="102"/>
@@ -13053,10 +13080,10 @@
         <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C5" s="381">
-        <f>('Main Page'!C5*'Main Page'!E5+'Main Page'!C6*'Main Page'!E6+'Main Page'!C7*'Main Page'!E7)/C11</f>
+        <f>('Main Page'!C5*'Main Page'!E5+'Main Page'!C6*'Main Page'!E6+'Main Page'!C7*'Main Page'!E7)/C13</f>
         <v>0</v>
       </c>
     </row>
@@ -13065,10 +13092,10 @@
         <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C6" s="381">
-        <f>('Main Page'!D5*'Main Page'!E5+'Main Page'!D6*'Main Page'!E6+'Main Page'!D7*'Main Page'!E7)/C11+'Main Page'!B46</f>
+        <f>('Main Page'!D5*'Main Page'!E5+'Main Page'!D6*'Main Page'!E6+'Main Page'!D7*'Main Page'!E7)/C13+'Main Page'!B46</f>
         <v>1.2043279805609703</v>
       </c>
       <c r="I6" s="103"/>
@@ -13080,7 +13107,7 @@
         <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C7" s="381">
         <f>'Main Page'!B9-'Main Page'!B46</f>
@@ -13095,7 +13122,7 @@
         <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C8" s="381">
         <f>'Main Page'!B46</f>
@@ -13107,10 +13134,10 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B9" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="C9" s="381">
         <f>-'Main Page'!B11</f>
@@ -13120,154 +13147,200 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B10" t="s">
-        <v>444</v>
+        <v>522</v>
       </c>
       <c r="C10" s="381">
         <f>-'Main Page'!B18</f>
         <v>0</v>
       </c>
       <c r="I10" s="103"/>
-      <c r="M10" s="358"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
+        <v>440</v>
+      </c>
+      <c r="B11" t="s">
+        <v>523</v>
+      </c>
+      <c r="C11" s="381">
+        <f>-'Main Page'!B18</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="103"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>440</v>
+      </c>
+      <c r="B12" t="s">
+        <v>524</v>
+      </c>
+      <c r="C12" s="381">
+        <f>-'Main Page'!B18</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="103"/>
+      <c r="M12" s="358"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
         <v>117</v>
       </c>
-      <c r="B11" t="s">
-        <v>474</v>
-      </c>
-      <c r="C11" s="381">
+      <c r="B13" t="s">
+        <v>470</v>
+      </c>
+      <c r="C13" s="381">
         <f>SUM('Main Page'!E5+'Main Page'!E6+'Main Page'!E7)</f>
         <v>20950.244259671897</v>
       </c>
-      <c r="I11" s="103"/>
-      <c r="M11" s="358"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" t="s">
+      <c r="I13" s="103"/>
+      <c r="M13" s="358"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
         <v>117</v>
       </c>
-      <c r="B12" t="s">
-        <v>446</v>
-      </c>
-      <c r="C12" s="381">
+      <c r="B14" t="s">
+        <v>442</v>
+      </c>
+      <c r="C14" s="381">
         <f>'Main Page'!E8</f>
         <v>6573.9348557027251</v>
       </c>
-      <c r="I12" s="103"/>
-      <c r="M12" s="358"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>431</v>
-      </c>
-      <c r="B13" t="s">
-        <v>447</v>
-      </c>
-      <c r="C13" s="381">
+      <c r="I14" s="103"/>
+      <c r="M14" s="358"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>429</v>
+      </c>
+      <c r="B15" t="s">
+        <v>443</v>
+      </c>
+      <c r="C15" s="381">
         <f>SUM('Main Page'!H5:H7)</f>
         <v>8623.1244137844569</v>
       </c>
-      <c r="I13" s="103"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" t="s">
-        <v>431</v>
-      </c>
-      <c r="B14" t="s">
-        <v>475</v>
-      </c>
-      <c r="C14" s="381">
+      <c r="I15" s="103"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>429</v>
+      </c>
+      <c r="B16" t="s">
+        <v>471</v>
+      </c>
+      <c r="C16" s="381">
         <f>SUM(GECdrivetrain!M11:'GECdrivetrain'!M12)/('Main Page'!$B$88)^2</f>
         <v>16.651119676874973</v>
       </c>
-      <c r="I14" s="103"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" t="s">
-        <v>431</v>
-      </c>
-      <c r="B15" t="s">
-        <v>448</v>
-      </c>
-      <c r="C15" s="381">
+      <c r="I16" s="103"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>429</v>
+      </c>
+      <c r="B17" t="s">
+        <v>444</v>
+      </c>
+      <c r="C17" s="381">
         <f>GECdrivetrain!M5</f>
         <v>5160.9544585651756</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
-        <v>430</v>
-      </c>
-      <c r="B16" t="s">
-        <v>476</v>
-      </c>
-      <c r="C16" s="393">
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>428</v>
+      </c>
+      <c r="B18" t="s">
+        <v>472</v>
+      </c>
+      <c r="C18" s="393">
         <f>'Main Page'!B19*100</f>
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
-      <c r="A17" t="s">
-        <v>430</v>
-      </c>
-      <c r="B17" t="s">
-        <v>477</v>
-      </c>
-      <c r="C17">
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>428</v>
+      </c>
+      <c r="B19" t="s">
+        <v>473</v>
+      </c>
+      <c r="C19">
         <f>'Main Page'!$B$88</f>
         <v>62.831853071795862</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
-      <c r="A18" t="s">
-        <v>479</v>
-      </c>
-      <c r="B18" t="s">
-        <v>478</v>
-      </c>
-      <c r="C18">
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>475</v>
+      </c>
+      <c r="B20" t="s">
+        <v>474</v>
+      </c>
+      <c r="C20">
         <f>'Main Page'!B14</f>
         <v>129646444.93189973</v>
       </c>
-      <c r="I18" s="103"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" t="s">
-        <v>480</v>
-      </c>
-      <c r="B19" t="s">
-        <v>481</v>
-      </c>
-      <c r="C19">
-        <f>2*'Main Page'!B15/100*SQRT(C18*'Main Page'!B16*C14*C17^2/('Main Page'!B16+C14*C17^2))</f>
+      <c r="I20" s="103"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>476</v>
+      </c>
+      <c r="B21" t="s">
+        <v>477</v>
+      </c>
+      <c r="C21">
+        <f>2*'Main Page'!B15/100*SQRT(C20*'Main Page'!B16*C16*C19^2/('Main Page'!B16+C16*C19^2))</f>
         <v>278494.4553663737</v>
       </c>
-      <c r="I19" s="103"/>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" t="s">
-        <v>482</v>
-      </c>
-      <c r="B20" t="s">
-        <v>483</v>
-      </c>
-      <c r="C20" s="333">
+      <c r="I21" s="103"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>478</v>
+      </c>
+      <c r="B22" t="s">
+        <v>479</v>
+      </c>
+      <c r="C22" s="333">
         <f>'Main Page'!B92*1000</f>
         <v>750000</v>
       </c>
-      <c r="M20" s="358"/>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="I21" s="103"/>
-      <c r="M21" s="358"/>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="I22" s="103"/>
       <c r="M22" s="358"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>430</v>
+      </c>
+      <c r="C23" s="18">
+        <f>'Main Page'!B13/2</f>
+        <v>25</v>
+      </c>
+      <c r="I23" s="103"/>
+      <c r="M23" s="358"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>431</v>
+      </c>
+      <c r="C24" s="18">
+        <f>'Main Page'!B56/2</f>
+        <v>1.25</v>
+      </c>
+      <c r="I24" s="103"/>
+      <c r="M24" s="358"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13276,10 +13349,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -13290,13 +13363,13 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" t="s">
         <v>427</v>
-      </c>
-      <c r="B1" t="s">
-        <v>428</v>
-      </c>
-      <c r="C1" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -13304,315 +13377,261 @@
         <v>385</v>
       </c>
       <c r="B3" t="s">
-        <v>484</v>
+        <v>518</v>
       </c>
       <c r="C3" s="103">
         <f>'Main Page'!B154*100</f>
         <v>3.4350000000000001</v>
       </c>
-      <c r="D3" s="103">
+    </row>
+    <row r="4" spans="1:14">
+      <c r="B4" t="s">
+        <v>519</v>
+      </c>
+      <c r="C4" s="103">
         <f>'Main Page'!B155*100</f>
         <v>3.4350000000000001</v>
       </c>
-      <c r="E3" s="103">
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
+      <c r="F4" s="103"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="B5" t="s">
+        <v>520</v>
+      </c>
+      <c r="C5" s="103">
         <f>'Main Page'!B156*100</f>
         <v>3.4350000000000001</v>
       </c>
-      <c r="F3" s="103">
+      <c r="D5" s="103"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
+      <c r="N5" s="358"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="B6" t="s">
+        <v>521</v>
+      </c>
+      <c r="C6" s="103">
         <f>'Main Page'!B157*100</f>
         <v>3.4350000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="B4" t="s">
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="N6" s="358"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="B7" t="s">
+        <v>480</v>
+      </c>
+      <c r="C7" t="s">
+        <v>486</v>
+      </c>
+      <c r="D7" t="s">
+        <v>481</v>
+      </c>
+      <c r="E7" t="s">
+        <v>482</v>
+      </c>
+      <c r="F7" t="s">
+        <v>483</v>
+      </c>
+      <c r="G7" t="s">
+        <v>484</v>
+      </c>
+      <c r="H7" t="s">
         <v>485</v>
       </c>
-      <c r="C4" t="s">
-        <v>491</v>
-      </c>
-      <c r="D4" t="s">
-        <v>486</v>
-      </c>
-      <c r="E4" t="s">
-        <v>487</v>
-      </c>
-      <c r="F4" t="s">
-        <v>488</v>
-      </c>
-      <c r="G4" t="s">
-        <v>489</v>
-      </c>
-      <c r="H4" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="C5" s="380">
+      <c r="N7" s="358"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="C8" s="380">
         <f>GECtwrdata!$B15/9</f>
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="D8">
         <f>GECtwrdata!$G15</f>
         <v>1456.5699814057803</v>
       </c>
-      <c r="E5" s="388">
+      <c r="E8" s="388">
         <f>GECtwrdata!$N15</f>
         <v>62126221909.368462</v>
       </c>
-      <c r="F5" s="388">
+      <c r="F8" s="388">
         <f>GECtwrdata!$N15</f>
         <v>62126221909.368462</v>
       </c>
-      <c r="G5" s="388">
+      <c r="G8" s="388">
         <f>GECtwrdata!$K15</f>
         <v>47789401468.744972</v>
       </c>
-      <c r="H5" s="388">
+      <c r="H8" s="388">
         <f>GECtwrdata!$H15</f>
         <v>35342917352.88517</v>
       </c>
-      <c r="N5" s="358"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="C6" s="380">
+      <c r="N8" s="358"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="C9" s="380">
         <f>GECtwrdata!$B16/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="D6">
+      <c r="D9">
         <f>GECtwrdata!$G16</f>
         <v>1319.6643913839366</v>
       </c>
-      <c r="E6" s="388">
+      <c r="E9" s="388">
         <f>GECtwrdata!$N16</f>
         <v>50601045349.013542</v>
       </c>
-      <c r="F6" s="388">
+      <c r="F9" s="388">
         <f>GECtwrdata!$N16</f>
         <v>50601045349.013542</v>
       </c>
-      <c r="G6" s="388">
+      <c r="G9" s="388">
         <f>GECtwrdata!$K16</f>
         <v>38923881037.702721</v>
       </c>
-      <c r="H6" s="388">
+      <c r="H9" s="388">
         <f>GECtwrdata!$H16</f>
         <v>32020974009.92263</v>
       </c>
-      <c r="N6" s="358"/>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="C7" s="380">
+      <c r="N9" s="358"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="C10" s="380">
         <f>GECtwrdata!$B17/9</f>
         <v>0.22222222222222221</v>
       </c>
-      <c r="D7">
+      <c r="D10">
         <f>GECtwrdata!$G17</f>
         <v>1189.4722103298889</v>
       </c>
-      <c r="E7" s="388">
+      <c r="E10" s="388">
         <f>GECtwrdata!$N17</f>
         <v>40756895137.180222</v>
       </c>
-      <c r="F7" s="388">
+      <c r="F10" s="388">
         <f>GECtwrdata!$N17</f>
         <v>40756895137.180222</v>
       </c>
-      <c r="G7" s="388">
+      <c r="G10" s="388">
         <f>GECtwrdata!$K17</f>
         <v>31351457797.830936</v>
       </c>
-      <c r="H7" s="388">
+      <c r="H10" s="388">
         <f>GECtwrdata!$H17</f>
         <v>28861928063.812893</v>
       </c>
-      <c r="N7" s="358"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="C8" s="380">
+      <c r="N10" s="358"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="C11" s="380">
         <f>GECtwrdata!$B18/9</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D8">
+      <c r="D11">
         <f>GECtwrdata!$G18</f>
         <v>1065.9934382436375</v>
       </c>
-      <c r="E8" s="388">
+      <c r="E11" s="388">
         <f>GECtwrdata!$N18</f>
         <v>32422036127.620483</v>
       </c>
-      <c r="F8" s="388">
+      <c r="F11" s="388">
         <f>GECtwrdata!$N18</f>
         <v>32422036127.620483</v>
       </c>
-      <c r="G8" s="388">
+      <c r="G11" s="388">
         <f>GECtwrdata!$K18</f>
         <v>24940027790.477295</v>
       </c>
-      <c r="H8" s="388">
+      <c r="H11" s="388">
         <f>GECtwrdata!$H18</f>
         <v>25865779514.555958</v>
       </c>
-      <c r="N8" s="358"/>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="C9" s="380">
+      <c r="N11" s="358"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="380">
         <f>GECtwrdata!$B19/9</f>
         <v>0.44444444444444442</v>
       </c>
-      <c r="D9">
+      <c r="D12">
         <f>GECtwrdata!$G19</f>
         <v>949.2280751251825</v>
       </c>
-      <c r="E9" s="388">
+      <c r="E12" s="388">
         <f>GECtwrdata!$N19</f>
         <v>25433971568.120796</v>
       </c>
-      <c r="F9" s="388">
+      <c r="F12" s="388">
         <f>GECtwrdata!$N19</f>
         <v>25433971568.120796</v>
       </c>
-      <c r="G9" s="388">
+      <c r="G12" s="388">
         <f>GECtwrdata!$K19</f>
         <v>19564593513.939072</v>
       </c>
-      <c r="H9" s="388">
+      <c r="H12" s="388">
         <f>GECtwrdata!$H19</f>
         <v>23032528362.151833</v>
       </c>
-      <c r="N9" s="358"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="C10" s="380">
+      <c r="N12" s="358"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13" s="380">
         <f>GECtwrdata!$B20/9</f>
         <v>0.55555555555555558</v>
       </c>
-      <c r="D10">
+      <c r="D13">
         <f>GECtwrdata!$G20</f>
         <v>839.17612097452354</v>
       </c>
-      <c r="E10" s="388">
+      <c r="E13" s="388">
         <f>GECtwrdata!$N20</f>
         <v>19639443100.502033</v>
       </c>
-      <c r="F10" s="388">
+      <c r="F13" s="388">
         <f>GECtwrdata!$N20</f>
         <v>19639443100.502033</v>
       </c>
-      <c r="G10" s="388">
+      <c r="G13" s="388">
         <f>GECtwrdata!$K20</f>
         <v>15107263923.4631</v>
       </c>
-      <c r="H10" s="388">
+      <c r="H13" s="388">
         <f>GECtwrdata!$H20</f>
         <v>20362174606.60051</v>
       </c>
-      <c r="N10" s="358"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="C11" s="380">
+      <c r="N13" s="358"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="C14" s="380">
         <f>GECtwrdata!$B21/9</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D11">
+      <c r="D14">
         <f>GECtwrdata!$G21</f>
         <v>735.83757579166081</v>
       </c>
-      <c r="E11" s="388">
+      <c r="E14" s="388">
         <f>GECtwrdata!$N21</f>
         <v>14894430760.619625</v>
       </c>
-      <c r="F11" s="388">
+      <c r="F14" s="388">
         <f>GECtwrdata!$N21</f>
         <v>14894430760.619625</v>
       </c>
-      <c r="G11" s="388">
+      <c r="G14" s="388">
         <f>GECtwrdata!$K21</f>
         <v>11457254431.245865</v>
       </c>
-      <c r="H11" s="388">
+      <c r="H14" s="388">
         <f>GECtwrdata!$H21</f>
         <v>17854718247.901989</v>
-      </c>
-      <c r="N11" s="358"/>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="C12" s="380">
-        <f>GECtwrdata!$B22/9</f>
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="D12">
-        <f>GECtwrdata!$G22</f>
-        <v>639.21243957659442</v>
-      </c>
-      <c r="E12" s="388">
-        <f>GECtwrdata!$N22</f>
-        <v>11064152978.363453</v>
-      </c>
-      <c r="F12" s="388">
-        <f>GECtwrdata!$N22</f>
-        <v>11064152978.363453</v>
-      </c>
-      <c r="G12" s="388">
-        <f>GECtwrdata!$K22</f>
-        <v>8510886906.433424</v>
-      </c>
-      <c r="H12" s="388">
-        <f>GECtwrdata!$H22</f>
-        <v>15510159286.056276</v>
-      </c>
-      <c r="N12" s="358"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="C13" s="380">
-        <f>GECtwrdata!$B23/9</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="D13">
-        <f>GECtwrdata!$G23</f>
-        <v>549.3007123293238</v>
-      </c>
-      <c r="E13" s="388">
-        <f>GECtwrdata!$N23</f>
-        <v>8023066577.657836</v>
-      </c>
-      <c r="F13" s="388">
-        <f>GECtwrdata!$N23</f>
-        <v>8023066577.657836</v>
-      </c>
-      <c r="G13" s="388">
-        <f>GECtwrdata!$K23</f>
-        <v>6171589675.1214123</v>
-      </c>
-      <c r="H13" s="388">
-        <f>GECtwrdata!$H23</f>
-        <v>13328497721.063362</v>
-      </c>
-      <c r="N13" s="358"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="C14" s="380">
-        <f>GECtwrdata!$B24/9</f>
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <f>GECtwrdata!$G24</f>
-        <v>466.10239404984969</v>
-      </c>
-      <c r="E14" s="388">
-        <f>GECtwrdata!$N24</f>
-        <v>5654866776.461628</v>
-      </c>
-      <c r="F14" s="388">
-        <f>GECtwrdata!$N24</f>
-        <v>5654866776.461628</v>
-      </c>
-      <c r="G14" s="388">
-        <f>GECtwrdata!$K24</f>
-        <v>4349897520.3550978</v>
-      </c>
-      <c r="H14" s="388">
-        <f>GECtwrdata!$H24</f>
-        <v>11309733552.923256</v>
       </c>
       <c r="I14" s="377"/>
       <c r="J14" s="377"/>
@@ -13621,7 +13640,83 @@
       <c r="N14" s="358"/>
     </row>
     <row r="15" spans="1:14">
+      <c r="C15" s="380">
+        <f>GECtwrdata!$B22/9</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="D15">
+        <f>GECtwrdata!$G22</f>
+        <v>639.21243957659442</v>
+      </c>
+      <c r="E15" s="388">
+        <f>GECtwrdata!$N22</f>
+        <v>11064152978.363453</v>
+      </c>
+      <c r="F15" s="388">
+        <f>GECtwrdata!$N22</f>
+        <v>11064152978.363453</v>
+      </c>
+      <c r="G15" s="388">
+        <f>GECtwrdata!$K22</f>
+        <v>8510886906.433424</v>
+      </c>
+      <c r="H15" s="388">
+        <f>GECtwrdata!$H22</f>
+        <v>15510159286.056276</v>
+      </c>
       <c r="N15" s="358"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="C16" s="380">
+        <f>GECtwrdata!$B23/9</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="D16">
+        <f>GECtwrdata!$G23</f>
+        <v>549.3007123293238</v>
+      </c>
+      <c r="E16" s="388">
+        <f>GECtwrdata!$N23</f>
+        <v>8023066577.657836</v>
+      </c>
+      <c r="F16" s="388">
+        <f>GECtwrdata!$N23</f>
+        <v>8023066577.657836</v>
+      </c>
+      <c r="G16" s="388">
+        <f>GECtwrdata!$K23</f>
+        <v>6171589675.1214123</v>
+      </c>
+      <c r="H16" s="388">
+        <f>GECtwrdata!$H23</f>
+        <v>13328497721.063362</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8">
+      <c r="C17" s="380">
+        <f>GECtwrdata!$B24/9</f>
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <f>GECtwrdata!$G24</f>
+        <v>466.10239404984969</v>
+      </c>
+      <c r="E17" s="388">
+        <f>GECtwrdata!$N24</f>
+        <v>5654866776.461628</v>
+      </c>
+      <c r="F17" s="388">
+        <f>GECtwrdata!$N24</f>
+        <v>5654866776.461628</v>
+      </c>
+      <c r="G17" s="388">
+        <f>GECtwrdata!$K24</f>
+        <v>4349897520.3550978</v>
+      </c>
+      <c r="H17" s="388">
+        <f>GECtwrdata!$H24</f>
+        <v>11309733552.923256</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>